<commit_message>
feat::wrench:change 药物 -> 个特
</commit_message>
<xml_diff>
--- a/template/NBS-final.result-批次号_产品编号.xlsx
+++ b/template/NBS-final.result-批次号_产品编号.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangyaoshen\GolandProjects\NB2xlsx\template\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE27E49-2FB0-42F9-8B4E-8707CE8437F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540" tabRatio="693" activeTab="8"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="693" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All variants data" sheetId="1" r:id="rId1"/>
     <sheet name="CNV" sheetId="2" r:id="rId2"/>
     <sheet name="补充实验" sheetId="3" r:id="rId3"/>
-    <sheet name="药物" sheetId="8" r:id="rId4"/>
+    <sheet name="个特" sheetId="8" r:id="rId4"/>
     <sheet name="基因ID" sheetId="9" r:id="rId5"/>
     <sheet name="QC" sheetId="4" r:id="rId6"/>
     <sheet name="样本信息" sheetId="5" r:id="rId7"/>
@@ -20,22 +26,22 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'All variants data'!$A$1:$CV$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CNV!$A$1:$AP$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">QC!$A$1:$P$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">补充实验!$A$1:$Q$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">药物!$A$1:$N$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">个特!$A$1:$N$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">基因ID!$A$1:$N$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">QC!$A$1:$P$1</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>作者</author>
   </authors>
   <commentList>
-    <comment ref="R1" authorId="0">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -47,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BC1" authorId="0">
+    <comment ref="BC1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000002000000}">
       <text>
         <r>
           <rPr>
@@ -667,15 +673,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="yyyy/m/d;@"/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="178" formatCode="yyyy/m/d;@"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -727,159 +729,21 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="41">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -894,13 +758,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.0999786370433668"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.396649067659536"/>
+        <fgColor theme="8" tint="0.3966490676595355"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -930,198 +794,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.149876400036622"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="0" tint="-0.1498458815271462"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1181,258 +859,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1467,7 +903,7 @@
     <xf numFmtId="14" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1522,58 +958,50 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1588,12 +1016,15 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="00FFFF00"/>
+      <color rgb="FFFFFF00"/>
     </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1880,101 +1311,100 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CV1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="$A2:$XFD8"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.90833333333333" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6333333333333" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.9083333333333" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.63333333333333" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.725" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="7.90833333333333" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="7.09166666666667" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="2" width="7.90625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.6328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7265625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="7.90625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="7.08984375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="9" max="10" width="7" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="7.09166666666667" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="7.09166666666667" style="1" customWidth="1"/>
-    <col min="13" max="13" width="8.09166666666667" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.0916666666667" style="1" customWidth="1"/>
-    <col min="15" max="16" width="11.725" style="1" customWidth="1"/>
-    <col min="17" max="17" width="10.725" style="1" customWidth="1"/>
-    <col min="18" max="18" width="8.63333333333333" style="1" customWidth="1"/>
-    <col min="19" max="19" width="10.6333333333333" style="1" customWidth="1"/>
-    <col min="20" max="20" width="9.63333333333333" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="15.6333333333333" style="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="8.90833333333333" style="1" customWidth="1"/>
-    <col min="23" max="23" width="10.6333333333333" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="8.45" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="7.08984375" style="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="7.08984375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8.08984375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.08984375" style="1" customWidth="1"/>
+    <col min="15" max="16" width="11.7265625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="10.7265625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="8.6328125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="10.6328125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="9.6328125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="15.6328125" style="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.90625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="10.6328125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="8.453125" style="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="11" style="1" customWidth="1"/>
-    <col min="26" max="27" width="10.6333333333333" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="28" max="28" width="11.725" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="30" width="10.6333333333333" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="16.725" style="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="10.9083333333333" style="1" customWidth="1"/>
-    <col min="33" max="33" width="10.6333333333333" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="34" max="36" width="15.6333333333333" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="37" max="48" width="10.6333333333333" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="49" max="49" width="13.0916666666667" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="50" max="50" width="12.45" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="51" max="51" width="12.725" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="52" max="52" width="13.3666666666667" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="53" max="59" width="7.09166666666667" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="27" width="10.6328125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="28" max="28" width="11.7265625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="30" width="10.6328125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="16.7265625" style="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="10.90625" style="1" customWidth="1"/>
+    <col min="33" max="33" width="10.6328125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="34" max="36" width="15.6328125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="37" max="48" width="10.6328125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="49" max="49" width="13.08984375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="50" max="50" width="12.453125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="51" max="51" width="12.7265625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="52" max="52" width="13.36328125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="53" max="59" width="7.08984375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="60" max="60" width="11" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="61" max="61" width="8.63333333333333" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="62" max="62" width="10.6333333333333" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="63" max="63" width="16.6333333333333" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="64" max="64" width="10.6333333333333" style="1" customWidth="1" collapsed="1"/>
-    <col min="65" max="65" width="9.45" style="1" customWidth="1"/>
-    <col min="66" max="66" width="8.90833333333333" style="1" customWidth="1"/>
-    <col min="67" max="68" width="8.90833333333333" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="69" max="69" width="9.45" style="1" customWidth="1" collapsed="1"/>
-    <col min="70" max="70" width="9.45" style="1" customWidth="1"/>
-    <col min="71" max="71" width="7.09166666666667" style="1" customWidth="1"/>
-    <col min="72" max="72" width="18.9083333333333" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="73" max="73" width="20.45" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="74" max="74" width="20.2666666666667" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="75" max="75" width="15.2666666666667" style="1" customWidth="1" collapsed="1"/>
-    <col min="76" max="76" width="18.3666666666667" style="1" customWidth="1"/>
-    <col min="77" max="77" width="21.6333333333333" style="1" customWidth="1"/>
-    <col min="78" max="79" width="17.9083333333333" style="1" customWidth="1"/>
-    <col min="80" max="80" width="16.9083333333333" style="1" customWidth="1"/>
-    <col min="81" max="82" width="14.9083333333333" style="1" customWidth="1"/>
-    <col min="83" max="83" width="19.2666666666667" style="1" customWidth="1"/>
-    <col min="84" max="84" width="19.2666666666667" customWidth="1"/>
-    <col min="85" max="85" width="27.725" style="1" customWidth="1"/>
-    <col min="86" max="86" width="17.6333333333333" style="1" customWidth="1"/>
-    <col min="87" max="87" width="15.6333333333333" style="1" customWidth="1"/>
-    <col min="88" max="88" width="16.0916666666667" style="1" customWidth="1"/>
-    <col min="89" max="89" width="18.0916666666667" style="1" customWidth="1"/>
-    <col min="90" max="90" width="16.3666666666667" style="1" customWidth="1"/>
-    <col min="91" max="91" width="12.6333333333333" style="1" customWidth="1"/>
-    <col min="92" max="92" width="12.0916666666667" style="1" customWidth="1"/>
-    <col min="93" max="93" width="12.6333333333333" style="1" customWidth="1"/>
-    <col min="94" max="94" width="11.45" style="1" customWidth="1"/>
-    <col min="95" max="95" width="12.3666666666667" customWidth="1"/>
-    <col min="96" max="96" width="13.45" customWidth="1"/>
-    <col min="97" max="97" width="11.0916666666667" customWidth="1"/>
-    <col min="98" max="98" width="12.6333333333333" customWidth="1"/>
-    <col min="99" max="99" width="11.6333333333333" customWidth="1"/>
-    <col min="100" max="100" width="15.0916666666667" customWidth="1"/>
+    <col min="61" max="61" width="8.6328125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="62" max="62" width="10.6328125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="63" max="63" width="16.6328125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="64" max="64" width="10.6328125" style="1" customWidth="1" collapsed="1"/>
+    <col min="65" max="65" width="9.453125" style="1" customWidth="1"/>
+    <col min="66" max="66" width="8.90625" style="1" customWidth="1"/>
+    <col min="67" max="68" width="8.90625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="69" max="69" width="9.453125" style="1" customWidth="1" collapsed="1"/>
+    <col min="70" max="70" width="9.453125" style="1" customWidth="1"/>
+    <col min="71" max="71" width="7.08984375" style="1" customWidth="1"/>
+    <col min="72" max="72" width="18.90625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="73" max="73" width="20.453125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="74" max="74" width="20.26953125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="75" max="75" width="15.26953125" style="1" customWidth="1" collapsed="1"/>
+    <col min="76" max="76" width="18.36328125" style="1" customWidth="1"/>
+    <col min="77" max="77" width="21.6328125" style="1" customWidth="1"/>
+    <col min="78" max="79" width="17.90625" style="1" customWidth="1"/>
+    <col min="80" max="80" width="16.90625" style="1" customWidth="1"/>
+    <col min="81" max="82" width="14.90625" style="1" customWidth="1"/>
+    <col min="83" max="83" width="19.26953125" style="1" customWidth="1"/>
+    <col min="84" max="84" width="19.26953125" customWidth="1"/>
+    <col min="85" max="85" width="27.7265625" style="1" customWidth="1"/>
+    <col min="86" max="86" width="17.6328125" style="1" customWidth="1"/>
+    <col min="87" max="87" width="15.6328125" style="1" customWidth="1"/>
+    <col min="88" max="88" width="16.08984375" style="1" customWidth="1"/>
+    <col min="89" max="89" width="18.08984375" style="1" customWidth="1"/>
+    <col min="90" max="90" width="16.36328125" style="1" customWidth="1"/>
+    <col min="91" max="91" width="12.6328125" style="1" customWidth="1"/>
+    <col min="92" max="92" width="12.08984375" style="1" customWidth="1"/>
+    <col min="93" max="93" width="12.6328125" style="1" customWidth="1"/>
+    <col min="94" max="94" width="11.453125" style="1" customWidth="1"/>
+    <col min="95" max="95" width="12.36328125" customWidth="1"/>
+    <col min="96" max="96" width="13.453125" customWidth="1"/>
+    <col min="97" max="97" width="11.08984375" customWidth="1"/>
+    <col min="98" max="98" width="12.6328125" customWidth="1"/>
+    <col min="99" max="99" width="11.6328125" customWidth="1"/>
+    <col min="100" max="100" width="15.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="31" customFormat="1" ht="15" spans="1:100">
+    <row r="1" spans="1:100" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
@@ -2277,74 +1707,70 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:CV1">
-    <extLst/>
-  </autoFilter>
+  <autoFilter ref="A1:CV1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CH$1:CH$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CH1:CH1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"P,LP,不报-验证为假,不报-合并后非烈性,不报-常见假点,不报-库内降级为VUS"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CK2:CK1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CK2:CK1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"正式报告,补充报告,正式报告-不报,补充报告-不报"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AP1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="$A2:$XFD12"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.45" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="2" max="2" width="8.63333333333333" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="18.6333333333333" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6333333333333" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.36666666666667" style="1" customWidth="1"/>
-    <col min="6" max="6" width="5.26666666666667" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.26666666666667" style="1" customWidth="1"/>
-    <col min="8" max="8" width="7.63333333333333" style="1" customWidth="1"/>
-    <col min="9" max="9" width="5.45" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.90833333333333" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7.90833333333333" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.725" style="1" customWidth="1"/>
-    <col min="13" max="13" width="16.0916666666667" style="1" customWidth="1"/>
-    <col min="14" max="14" width="14.725" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15.0916666666667" style="1" customWidth="1"/>
-    <col min="16" max="16" width="15.3666666666667" style="1" customWidth="1"/>
-    <col min="17" max="17" width="12.725" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.3666666666667" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="19" width="11.6333333333333" style="1" customWidth="1"/>
-    <col min="20" max="20" width="10.6333333333333" style="1" customWidth="1"/>
-    <col min="21" max="21" width="5.45" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="24" width="3.36666666666667" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="25" max="25" width="10.6333333333333" style="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="31" width="10.6333333333333" style="1" customWidth="1"/>
-    <col min="32" max="32" width="11.6333333333333" style="1" customWidth="1"/>
-    <col min="33" max="33" width="13.45" style="1" customWidth="1"/>
-    <col min="34" max="34" width="10.3666666666667" style="1" customWidth="1"/>
-    <col min="35" max="35" width="15.6333333333333" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="36" max="36" width="15.6333333333333" style="1" customWidth="1"/>
-    <col min="37" max="37" width="10.6333333333333" style="1" customWidth="1"/>
-    <col min="38" max="38" width="15.6333333333333" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="39" max="39" width="15.6333333333333" style="1" customWidth="1"/>
-    <col min="40" max="40" width="10.6333333333333" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.453125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="2" width="8.6328125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="18.6328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5.36328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.26953125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.26953125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6328125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="5.453125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.90625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.90625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7265625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="16.08984375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7265625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.08984375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15.36328125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.7265625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.36328125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="11.6328125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="10.6328125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="5.453125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="24" width="3.36328125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="25" max="25" width="10.6328125" style="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="31" width="10.6328125" style="1" customWidth="1"/>
+    <col min="32" max="32" width="11.6328125" style="1" customWidth="1"/>
+    <col min="33" max="33" width="13.453125" style="1" customWidth="1"/>
+    <col min="34" max="34" width="10.36328125" style="1" customWidth="1"/>
+    <col min="35" max="35" width="15.6328125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="36" max="36" width="15.6328125" style="1" customWidth="1"/>
+    <col min="37" max="37" width="10.6328125" style="1" customWidth="1"/>
+    <col min="38" max="38" width="15.6328125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="39" max="39" width="15.6328125" style="1" customWidth="1"/>
+    <col min="40" max="40" width="10.6328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2473,60 +1899,56 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AP1">
-    <extLst/>
-  </autoFilter>
+  <autoFilter ref="A1:AP1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB1" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"补充报告,正式报告"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD1" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Hom,Het,Hemi"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE1" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"A,B"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF1" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"Pathogenic,Likely pathogenic,VUS"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="$A2:$XFD17"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.725" customWidth="1" outlineLevel="1"/>
-    <col min="2" max="2" width="10.45" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="18.6333333333333" customWidth="1"/>
-    <col min="4" max="4" width="14.6333333333333" customWidth="1"/>
-    <col min="6" max="6" width="15.6333333333333" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="17.3666666666667" customWidth="1" outlineLevel="1"/>
+    <col min="1" max="1" width="7.7265625" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="2" width="10.453125" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="18.6328125" customWidth="1"/>
+    <col min="4" max="4" width="14.6328125" customWidth="1"/>
+    <col min="6" max="6" width="15.6328125" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="17.36328125" customWidth="1" outlineLevel="1"/>
     <col min="8" max="8" width="15" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="17.2666666666667" customWidth="1"/>
-    <col min="10" max="10" width="16.2666666666667" customWidth="1"/>
-    <col min="11" max="12" width="15.6333333333333" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="21.3666666666667" customWidth="1"/>
-    <col min="14" max="14" width="27.0916666666667" customWidth="1"/>
-    <col min="15" max="15" width="23.725" customWidth="1"/>
-    <col min="16" max="16" width="11.0916666666667" customWidth="1"/>
+    <col min="9" max="9" width="17.26953125" customWidth="1"/>
+    <col min="10" max="10" width="16.26953125" customWidth="1"/>
+    <col min="11" max="12" width="15.6328125" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="13" width="21.36328125" customWidth="1"/>
+    <col min="14" max="14" width="27.08984375" customWidth="1"/>
+    <col min="15" max="15" width="23.7265625" customWidth="1"/>
+    <col min="16" max="16" width="11.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
@@ -2586,41 +2008,38 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q1">
-    <extLst/>
-  </autoFilter>
+  <autoFilter ref="A1:Q1" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.09166666666667" customWidth="1"/>
-    <col min="2" max="2" width="14.45" customWidth="1"/>
-    <col min="3" max="3" width="19.9083333333333" customWidth="1"/>
-    <col min="4" max="4" width="11.725" customWidth="1"/>
+    <col min="1" max="1" width="9.08984375" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="3" max="3" width="19.90625" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="10.725" customWidth="1"/>
-    <col min="8" max="8" width="15.45" customWidth="1"/>
-    <col min="9" max="9" width="13.6333333333333" customWidth="1"/>
-    <col min="10" max="10" width="17.6333333333333" customWidth="1"/>
+    <col min="7" max="7" width="10.7265625" customWidth="1"/>
+    <col min="8" max="8" width="15.453125" customWidth="1"/>
+    <col min="9" max="9" width="13.6328125" customWidth="1"/>
+    <col min="10" max="10" width="17.6328125" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="11.2666666666667" customWidth="1"/>
-    <col min="13" max="13" width="11.45" customWidth="1"/>
-    <col min="14" max="14" width="12.6333333333333" customWidth="1"/>
+    <col min="12" max="12" width="11.26953125" customWidth="1"/>
+    <col min="13" max="13" width="11.453125" customWidth="1"/>
+    <col min="14" max="14" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="26" customFormat="1" spans="1:14">
+    <row r="1" spans="1:14" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
@@ -2665,39 +2084,36 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N1">
-    <extLst/>
-  </autoFilter>
+  <autoFilter ref="A1:N1" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="$A2:$XFD7"/>
+      <selection activeCell="A7" sqref="A2:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.90833333333333" customWidth="1"/>
-    <col min="2" max="2" width="11.0916666666667" customWidth="1"/>
-    <col min="3" max="3" width="20.6333333333333" customWidth="1"/>
-    <col min="4" max="4" width="11.45" customWidth="1"/>
+    <col min="1" max="1" width="8.90625" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
-    <col min="6" max="6" width="9.90833333333333" customWidth="1"/>
-    <col min="10" max="10" width="9.90833333333333" customWidth="1"/>
-    <col min="11" max="11" width="12.9083333333333" customWidth="1"/>
-    <col min="12" max="12" width="10.725" customWidth="1"/>
-    <col min="13" max="13" width="16.725" customWidth="1"/>
+    <col min="6" max="6" width="9.90625" customWidth="1"/>
+    <col min="10" max="10" width="9.90625" customWidth="1"/>
+    <col min="11" max="11" width="12.90625" customWidth="1"/>
+    <col min="12" max="12" width="10.7265625" customWidth="1"/>
+    <col min="13" max="13" width="16.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2742,41 +2158,38 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N1">
-    <extLst/>
-  </autoFilter>
+  <autoFilter ref="A1:N1" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G2" sqref="$A2:$XFD17"/>
+      <selection activeCell="G2" sqref="A2:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.26666666666667" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.725" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" style="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.36666666666667" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.3666666666667" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.725" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.0916666666667" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.9083333333333" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.36328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.36328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7265625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.08984375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.90625" style="1" customWidth="1"/>
     <col min="9" max="9" width="34" style="1" customWidth="1"/>
     <col min="10" max="10" width="47" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.3666666666667" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.9083333333333" style="1" customWidth="1"/>
-    <col min="13" max="15" width="10.6333333333333" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.36328125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.90625" style="1" customWidth="1"/>
+    <col min="13" max="15" width="10.6328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>148</v>
       </c>
@@ -2824,36 +2237,33 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P1">
-    <extLst/>
-  </autoFilter>
+  <autoFilter ref="A1:P1" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:CJ35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.0916666666667" customWidth="1"/>
-    <col min="2" max="2" width="11.3666666666667" customWidth="1"/>
-    <col min="3" max="3" width="11.725" customWidth="1"/>
-    <col min="6" max="6" width="14.0916666666667" customWidth="1"/>
-    <col min="7" max="7" width="12.0916666666667" customWidth="1"/>
+    <col min="1" max="1" width="11.08984375" customWidth="1"/>
+    <col min="2" max="2" width="11.36328125" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" customWidth="1"/>
+    <col min="6" max="6" width="14.08984375" customWidth="1"/>
+    <col min="7" max="7" width="12.08984375" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="11.2666666666667" customWidth="1"/>
+    <col min="10" max="10" width="11.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:88">
+    <row r="1" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A1" s="21"/>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -2943,7 +2353,7 @@
       <c r="CI1" s="21"/>
       <c r="CJ1" s="21"/>
     </row>
-    <row r="2" s="20" customFormat="1" ht="20.25" customHeight="1" spans="1:88">
+    <row r="2" spans="1:88" s="20" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -3033,7 +2443,7 @@
       <c r="CI2" s="24"/>
       <c r="CJ2" s="24"/>
     </row>
-    <row r="3" spans="1:88">
+    <row r="3" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A3" s="21"/>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
@@ -3123,7 +2533,7 @@
       <c r="CI3" s="21"/>
       <c r="CJ3" s="21"/>
     </row>
-    <row r="4" spans="1:88">
+    <row r="4" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A4" s="21"/>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
@@ -3213,7 +2623,7 @@
       <c r="CI4" s="21"/>
       <c r="CJ4" s="21"/>
     </row>
-    <row r="5" spans="1:88">
+    <row r="5" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A5" s="21"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
@@ -3303,7 +2713,7 @@
       <c r="CI5" s="21"/>
       <c r="CJ5" s="21"/>
     </row>
-    <row r="6" spans="1:88">
+    <row r="6" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
@@ -3393,7 +2803,7 @@
       <c r="CI6" s="21"/>
       <c r="CJ6" s="21"/>
     </row>
-    <row r="7" spans="1:88">
+    <row r="7" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
@@ -3483,7 +2893,7 @@
       <c r="CI7" s="21"/>
       <c r="CJ7" s="21"/>
     </row>
-    <row r="8" spans="1:88">
+    <row r="8" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A8" s="21"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
@@ -3573,7 +2983,7 @@
       <c r="CI8" s="21"/>
       <c r="CJ8" s="21"/>
     </row>
-    <row r="9" spans="1:88">
+    <row r="9" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
@@ -3663,7 +3073,7 @@
       <c r="CI9" s="21"/>
       <c r="CJ9" s="21"/>
     </row>
-    <row r="10" spans="1:88">
+    <row r="10" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
@@ -3753,7 +3163,7 @@
       <c r="CI10" s="21"/>
       <c r="CJ10" s="21"/>
     </row>
-    <row r="11" spans="1:88">
+    <row r="11" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
@@ -3843,7 +3253,7 @@
       <c r="CI11" s="21"/>
       <c r="CJ11" s="21"/>
     </row>
-    <row r="12" spans="1:88">
+    <row r="12" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
       <c r="B12" s="21"/>
       <c r="C12" s="21"/>
@@ -3933,7 +3343,7 @@
       <c r="CI12" s="21"/>
       <c r="CJ12" s="21"/>
     </row>
-    <row r="13" spans="1:88">
+    <row r="13" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A13" s="21"/>
       <c r="B13" s="21"/>
       <c r="C13" s="21"/>
@@ -4023,7 +3433,7 @@
       <c r="CI13" s="21"/>
       <c r="CJ13" s="21"/>
     </row>
-    <row r="14" spans="1:88">
+    <row r="14" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
@@ -4113,7 +3523,7 @@
       <c r="CI14" s="21"/>
       <c r="CJ14" s="21"/>
     </row>
-    <row r="15" spans="1:88">
+    <row r="15" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A15" s="21"/>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
@@ -4203,7 +3613,7 @@
       <c r="CI15" s="21"/>
       <c r="CJ15" s="21"/>
     </row>
-    <row r="16" spans="1:88">
+    <row r="16" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A16" s="21"/>
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
@@ -4293,7 +3703,7 @@
       <c r="CI16" s="21"/>
       <c r="CJ16" s="21"/>
     </row>
-    <row r="17" spans="1:88">
+    <row r="17" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A17" s="21"/>
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
@@ -4383,7 +3793,7 @@
       <c r="CI17" s="21"/>
       <c r="CJ17" s="21"/>
     </row>
-    <row r="18" spans="1:88">
+    <row r="18" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A18" s="21"/>
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
@@ -4473,7 +3883,7 @@
       <c r="CI18" s="21"/>
       <c r="CJ18" s="21"/>
     </row>
-    <row r="19" spans="1:88">
+    <row r="19" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
       <c r="B19" s="21"/>
       <c r="C19" s="21"/>
@@ -4563,7 +3973,7 @@
       <c r="CI19" s="21"/>
       <c r="CJ19" s="21"/>
     </row>
-    <row r="20" spans="1:88">
+    <row r="20" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A20" s="21"/>
       <c r="B20" s="21"/>
       <c r="C20" s="21"/>
@@ -4653,7 +4063,7 @@
       <c r="CI20" s="21"/>
       <c r="CJ20" s="21"/>
     </row>
-    <row r="21" spans="1:88">
+    <row r="21" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
@@ -4743,7 +4153,7 @@
       <c r="CI21" s="21"/>
       <c r="CJ21" s="21"/>
     </row>
-    <row r="22" spans="1:88">
+    <row r="22" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A22" s="21"/>
       <c r="B22" s="21"/>
       <c r="C22" s="21"/>
@@ -4833,7 +4243,7 @@
       <c r="CI22" s="21"/>
       <c r="CJ22" s="21"/>
     </row>
-    <row r="23" spans="1:88">
+    <row r="23" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A23" s="21"/>
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
@@ -4923,7 +4333,7 @@
       <c r="CI23" s="21"/>
       <c r="CJ23" s="21"/>
     </row>
-    <row r="24" spans="1:88">
+    <row r="24" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A24" s="21"/>
       <c r="B24" s="21"/>
       <c r="C24" s="21"/>
@@ -5013,7 +4423,7 @@
       <c r="CI24" s="21"/>
       <c r="CJ24" s="21"/>
     </row>
-    <row r="25" spans="1:88">
+    <row r="25" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A25" s="21"/>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
@@ -5103,7 +4513,7 @@
       <c r="CI25" s="21"/>
       <c r="CJ25" s="21"/>
     </row>
-    <row r="26" spans="1:88">
+    <row r="26" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A26" s="21"/>
       <c r="B26" s="21"/>
       <c r="C26" s="21"/>
@@ -5193,7 +4603,7 @@
       <c r="CI26" s="21"/>
       <c r="CJ26" s="21"/>
     </row>
-    <row r="27" spans="1:88">
+    <row r="27" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A27" s="21"/>
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
@@ -5283,7 +4693,7 @@
       <c r="CI27" s="21"/>
       <c r="CJ27" s="21"/>
     </row>
-    <row r="28" spans="1:88">
+    <row r="28" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A28" s="21"/>
       <c r="B28" s="21"/>
       <c r="C28" s="21"/>
@@ -5373,7 +4783,7 @@
       <c r="CI28" s="21"/>
       <c r="CJ28" s="21"/>
     </row>
-    <row r="29" spans="1:88">
+    <row r="29" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A29" s="21"/>
       <c r="B29" s="21"/>
       <c r="C29" s="21"/>
@@ -5463,7 +4873,7 @@
       <c r="CI29" s="21"/>
       <c r="CJ29" s="21"/>
     </row>
-    <row r="30" spans="1:88">
+    <row r="30" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A30" s="21"/>
       <c r="B30" s="21"/>
       <c r="C30" s="21"/>
@@ -5553,7 +4963,7 @@
       <c r="CI30" s="21"/>
       <c r="CJ30" s="21"/>
     </row>
-    <row r="31" spans="1:88">
+    <row r="31" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
@@ -5643,7 +5053,7 @@
       <c r="CI31" s="21"/>
       <c r="CJ31" s="21"/>
     </row>
-    <row r="32" spans="1:88">
+    <row r="32" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A32" s="21"/>
       <c r="B32" s="21"/>
       <c r="C32" s="21"/>
@@ -5733,7 +5143,7 @@
       <c r="CI32" s="21"/>
       <c r="CJ32" s="21"/>
     </row>
-    <row r="33" spans="1:88">
+    <row r="33" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
@@ -5823,7 +5233,7 @@
       <c r="CI33" s="21"/>
       <c r="CJ33" s="21"/>
     </row>
-    <row r="34" spans="1:88">
+    <row r="34" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A34" s="21"/>
       <c r="B34" s="21"/>
       <c r="C34" s="21"/>
@@ -5913,7 +5323,7 @@
       <c r="CI34" s="21"/>
       <c r="CJ34" s="21"/>
     </row>
-    <row r="35" spans="1:88">
+    <row r="35" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
       <c r="C35" s="21"/>
@@ -6004,55 +5414,53 @@
       <c r="CJ35" s="21"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z1:Z2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z1:Z2" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>"有,无"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <sheetData/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Y7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.45" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.9083333333333" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.725" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.3666666666667" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6333333333333" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.2666666666667" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.45" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.2666666666667" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.90625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.26953125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="24" customHeight="1" spans="1:25">
+    <row r="1" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>161</v>
       </c>
@@ -6127,42 +5535,42 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="E2" s="8"/>
       <c r="F2" s="9"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="E3" s="8"/>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="E4" s="8"/>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="E5" s="8"/>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="E6" s="8"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -6170,20 +5578,20 @@
       <c r="F7" s="9"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="0" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="14"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="15"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="16"/>
     <cfRule type="duplicateValues" dxfId="0" priority="17"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X1" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat::wrench:update template for 个特 and 基因ID
</commit_message>
<xml_diff>
--- a/template/NBS-final.result-批次号_产品编号.xlsx
+++ b/template/NBS-final.result-批次号_产品编号.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangyaoshen\GolandProjects\NB2xlsx\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE27E49-2FB0-42F9-8B4E-8707CE8437F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF01CF7D-FD46-4F7A-AD49-E2D7BC0F4187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="693" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15990" tabRatio="693" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All variants data" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="196">
   <si>
     <t>期数</t>
   </si>
@@ -532,9 +532,6 @@
     <t>F8int22h-10.8k&amp;12k最终结果</t>
   </si>
   <si>
-    <t>药物名称</t>
-  </si>
-  <si>
     <t>检测基因</t>
   </si>
   <si>
@@ -542,21 +539,6 @@
   </si>
   <si>
     <t>检测结果</t>
-  </si>
-  <si>
-    <t>用药建议</t>
-  </si>
-  <si>
-    <t>结果说明</t>
-  </si>
-  <si>
-    <t>药物类别</t>
-  </si>
-  <si>
-    <t>total reads</t>
-  </si>
-  <si>
-    <t>序号</t>
   </si>
   <si>
     <t>Order</t>
@@ -668,6 +650,60 @@
   <si>
     <t>发送报告内部周期
 （2017.8.21起）</t>
+  </si>
+  <si>
+    <t>rs</t>
+  </si>
+  <si>
+    <t>SNP ID</t>
+  </si>
+  <si>
+    <t>基因型</t>
+  </si>
+  <si>
+    <t>Total Depth</t>
+  </si>
+  <si>
+    <t>是否通过质控</t>
+  </si>
+  <si>
+    <t>个特分类</t>
+  </si>
+  <si>
+    <t>个特名称</t>
+  </si>
+  <si>
+    <t>个特ID</t>
+  </si>
+  <si>
+    <t>个特简介</t>
+  </si>
+  <si>
+    <t>位点所在染色体</t>
+  </si>
+  <si>
+    <t>基因名称</t>
+  </si>
+  <si>
+    <t>基因型结果</t>
+  </si>
+  <si>
+    <t>基因型频率</t>
+  </si>
+  <si>
+    <t>基因型组合频率</t>
+  </si>
+  <si>
+    <t>结果解读</t>
+  </si>
+  <si>
+    <t>Total depth&amp;A.ratio</t>
+  </si>
+  <si>
+    <t>低质量位点个数</t>
+  </si>
+  <si>
+    <t>待验证位点</t>
   </si>
 </sst>
 </file>
@@ -675,7 +711,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="yyyy/m/d;@"/>
+    <numFmt numFmtId="176" formatCode="yyyy/m/d;@"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -743,7 +779,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -795,6 +831,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.1498458815271462"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79995117038483843"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -863,12 +911,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -903,7 +951,7 @@
     <xf numFmtId="14" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -929,7 +977,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -957,6 +1004,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1404,305 +1454,305 @@
     <col min="100" max="100" width="15.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:100" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:100" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="I1" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="K1" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="L1" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="M1" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="32" t="s">
+      <c r="N1" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="32" t="s">
+      <c r="O1" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="32" t="s">
+      <c r="P1" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="32" t="s">
+      <c r="Q1" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="32" t="s">
+      <c r="R1" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="32" t="s">
+      <c r="S1" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="32" t="s">
+      <c r="T1" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="32" t="s">
+      <c r="U1" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="32" t="s">
+      <c r="V1" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="32" t="s">
+      <c r="W1" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="32" t="s">
+      <c r="X1" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="32" t="s">
+      <c r="Y1" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="32" t="s">
+      <c r="Z1" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="32" t="s">
+      <c r="AA1" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="32" t="s">
+      <c r="AB1" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="32" t="s">
+      <c r="AC1" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="32" t="s">
+      <c r="AD1" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="32" t="s">
+      <c r="AE1" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="32" t="s">
+      <c r="AF1" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="32" t="s">
+      <c r="AG1" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="32" t="s">
+      <c r="AH1" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="32" t="s">
+      <c r="AI1" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="32" t="s">
+      <c r="AJ1" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="32" t="s">
+      <c r="AK1" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="32" t="s">
+      <c r="AL1" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="32" t="s">
+      <c r="AM1" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="32" t="s">
+      <c r="AN1" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="32" t="s">
+      <c r="AO1" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="32" t="s">
+      <c r="AP1" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="32" t="s">
+      <c r="AQ1" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="32" t="s">
+      <c r="AR1" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="32" t="s">
+      <c r="AS1" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="32" t="s">
+      <c r="AT1" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="32" t="s">
+      <c r="AU1" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="32" t="s">
+      <c r="AV1" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="32" t="s">
+      <c r="AW1" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="32" t="s">
+      <c r="AX1" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="32" t="s">
+      <c r="AY1" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="32" t="s">
+      <c r="AZ1" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="32" t="s">
+      <c r="BA1" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="32" t="s">
+      <c r="BB1" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="32" t="s">
+      <c r="BC1" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="32" t="s">
+      <c r="BD1" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="32" t="s">
+      <c r="BE1" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" s="32" t="s">
+      <c r="BF1" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="32" t="s">
+      <c r="BG1" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="32" t="s">
+      <c r="BH1" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" s="32" t="s">
+      <c r="BI1" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" s="32" t="s">
+      <c r="BJ1" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" s="32" t="s">
+      <c r="BK1" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" s="32" t="s">
+      <c r="BL1" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" s="32" t="s">
+      <c r="BM1" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" s="32" t="s">
+      <c r="BN1" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" s="32" t="s">
+      <c r="BO1" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" s="32" t="s">
+      <c r="BP1" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" s="32" t="s">
+      <c r="BQ1" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" s="32" t="s">
+      <c r="BR1" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="BS1" s="32" t="s">
+      <c r="BS1" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="BT1" s="32" t="s">
+      <c r="BT1" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="BU1" s="32" t="s">
+      <c r="BU1" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="BV1" s="32" t="s">
+      <c r="BV1" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="BW1" s="32" t="s">
+      <c r="BW1" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="BX1" s="32" t="s">
+      <c r="BX1" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="BY1" s="32" t="s">
+      <c r="BY1" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="BZ1" s="32" t="s">
+      <c r="BZ1" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="CA1" s="32" t="s">
+      <c r="CA1" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="CB1" s="32" t="s">
+      <c r="CB1" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="CC1" s="32" t="s">
+      <c r="CC1" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="CD1" s="32" t="s">
+      <c r="CD1" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="CE1" s="33" t="s">
+      <c r="CE1" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="CF1" s="33" t="s">
+      <c r="CF1" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="CG1" s="32" t="s">
+      <c r="CG1" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="CH1" s="34" t="s">
+      <c r="CH1" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="CI1" s="32" t="s">
+      <c r="CI1" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="CJ1" s="35" t="s">
+      <c r="CJ1" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="CK1" s="32" t="s">
+      <c r="CK1" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="CL1" s="32" t="s">
+      <c r="CL1" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="CM1" s="32" t="s">
+      <c r="CM1" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="CN1" s="32" t="s">
+      <c r="CN1" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="CO1" s="32" t="s">
+      <c r="CO1" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="CP1" s="32" t="s">
+      <c r="CP1" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="CQ1" s="31" t="s">
+      <c r="CQ1" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="CR1" s="31" t="s">
+      <c r="CR1" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="CS1" s="36" t="s">
+      <c r="CS1" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="CT1" s="31" t="s">
+      <c r="CT1" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="CU1" s="36" t="s">
+      <c r="CU1" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="CV1" s="31" t="s">
+      <c r="CV1" s="30" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1789,10 +1839,10 @@
       <c r="F1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="28" t="s">
         <v>104</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -1813,13 +1863,13 @@
       <c r="N1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="O1" s="30" t="s">
+      <c r="O1" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="30" t="s">
+      <c r="P1" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="Q1" s="30" t="s">
+      <c r="Q1" s="29" t="s">
         <v>90</v>
       </c>
       <c r="R1" s="1" t="s">
@@ -1852,13 +1902,13 @@
       <c r="AA1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="AB1" s="29" t="s">
+      <c r="AB1" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="AC1" s="29" t="s">
+      <c r="AC1" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="AD1" s="29" t="s">
+      <c r="AD1" s="28" t="s">
         <v>122</v>
       </c>
       <c r="AE1" s="1" t="s">
@@ -1949,55 +1999,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="J1" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="M1" s="28" t="s">
+      <c r="M1" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="N1" s="28" t="s">
+      <c r="N1" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="O1" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="P1" s="27" t="s">
+      <c r="P1" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="Q1" s="27" t="s">
+      <c r="Q1" s="26" t="s">
         <v>93</v>
       </c>
       <c r="R1" t="s">
@@ -2016,11 +2066,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2039,48 +2087,72 @@
     <col min="14" max="14" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:22" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="26" t="s">
-        <v>139</v>
-      </c>
-      <c r="G1" s="26" t="s">
+      <c r="F1" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>185</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="J1" s="37" t="s">
+        <v>187</v>
+      </c>
+      <c r="K1" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="L1" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="M1" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="N1" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="O1" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="P1" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="I1" s="26" t="s">
-        <v>142</v>
-      </c>
-      <c r="J1" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="K1" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="L1" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="26" t="s">
-        <v>145</v>
+      <c r="Q1" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="R1" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="S1" s="38" t="s">
+        <v>194</v>
+      </c>
+      <c r="T1" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="U1" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="37" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2095,9 +2167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A2:XFD7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2111,50 +2181,51 @@
     <col min="11" max="11" width="12.90625" customWidth="1"/>
     <col min="12" max="12" width="10.7265625" customWidth="1"/>
     <col min="13" max="13" width="16.7265625" customWidth="1"/>
+    <col min="14" max="14" width="15.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="25" t="s">
+      <c r="K1" t="s">
+        <v>180</v>
+      </c>
+      <c r="L1" t="s">
+        <v>181</v>
+      </c>
+      <c r="M1" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="25" t="s">
-        <v>146</v>
-      </c>
       <c r="N1" s="25" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -2191,40 +2262,40 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>91</v>
@@ -2233,7 +2304,7 @@
         <v>93</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -5462,77 +5533,77 @@
   <sheetData>
     <row r="1" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="I1" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="J1" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="K1" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="M1" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="N1" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="O1" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>169</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>175</v>
       </c>
       <c r="Q1" s="11"/>
       <c r="R1" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="S1" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="T1" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="U1" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="V1" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="W1" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="X1" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="Y1" s="19" t="s">
         <v>177</v>
-      </c>
-      <c r="T1" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="U1" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="V1" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="W1" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="X1" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="Y1" s="19" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat:add pre_class,pre_pro,报告到期日 into template
</commit_message>
<xml_diff>
--- a/template/NBS-final.result-批次号_产品编号.xlsx
+++ b/template/NBS-final.result-批次号_产品编号.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tianlin\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C501D9E6-2964-4E03-93C9-2E3CDE83BBC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="693" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28800" windowHeight="12540" tabRatio="693"/>
   </bookViews>
   <sheets>
     <sheet name="All variants data" sheetId="1" r:id="rId1"/>
@@ -26,42 +20,40 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'All variants data'!$A$1:$CV$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CNV!$A$1:$AP$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">QC!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">补充实验!$A$1:$S$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">个特!$A$1:$V$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">基因ID!$A$1:$N$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">任务单!$A$1:$Y$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">QC!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>作者</author>
   </authors>
   <commentList>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
+    <comment ref="R1" authorId="0">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>PGD-单基因：必须提供单基因遗传病的致病基因</t>
         </r>
       </text>
     </comment>
-    <comment ref="BC1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000002000000}">
+    <comment ref="BC1" authorId="0">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>说明:
@@ -74,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="205">
   <si>
     <t>期数</t>
   </si>
@@ -262,7 +254,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -274,7 +265,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -309,7 +299,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -321,7 +310,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -422,6 +410,12 @@
     <t>是否新增解读</t>
   </si>
   <si>
+    <t>pre_class</t>
+  </si>
+  <si>
+    <t>pre_pro</t>
+  </si>
+  <si>
     <t>#sample</t>
   </si>
   <si>
@@ -654,6 +648,9 @@
   </si>
   <si>
     <t>产品编号</t>
+  </si>
+  <si>
+    <t>报告到期日</t>
   </si>
   <si>
     <t>分配日期</t>
@@ -734,11 +731,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="5">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="yyyy/m/d;@"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -751,7 +752,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -759,7 +759,6 @@
       <b/>
       <sz val="9"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -767,35 +766,30 @@
       <sz val="9"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="10.5"/>
       <color indexed="8"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -803,14 +797,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -818,7 +810,13 @@
       <sz val="11"/>
       <color rgb="FF201F1E"/>
       <name val="宋体"/>
-      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
@@ -826,23 +824,159 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="12">
+  <fills count="43">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -857,13 +991,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <fgColor theme="2" tint="-0.0999786370433668"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.3966490676595355"/>
+        <fgColor theme="8" tint="0.396649067659536"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -881,13 +1015,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79992065187536243"/>
+        <fgColor theme="8" tint="0.799920651875362"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39994506668294322"/>
+        <fgColor theme="5" tint="0.399945066682943"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -905,12 +1039,198 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14981536301767021"/>
+        <fgColor theme="0" tint="-0.14981536301767"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -970,11 +1290,253 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1050,6 +1612,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1075,58 +1640,66 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1141,16 +1714,13 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FFFFFF00"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="00FFFF00"/>
+      <color rgb="00FF0000"/>
     </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1437,22 +2007,23 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CV1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:CX1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomRight" activeCell="CY7" sqref="CY7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="8" style="1" customWidth="1"/>
     <col min="2" max="2" width="7.875" style="1" customWidth="1"/>
@@ -1530,336 +2101,346 @@
     <col min="100" max="100" width="15.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:100" s="37" customFormat="1" ht="15" x14ac:dyDescent="0.15">
-      <c r="A1" s="38" t="s">
+    <row r="1" s="38" customFormat="1" ht="15" spans="1:102">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="H1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="I1" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="J1" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="38" t="s">
+      <c r="K1" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="38" t="s">
+      <c r="L1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="38" t="s">
+      <c r="M1" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="38" t="s">
+      <c r="N1" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="38" t="s">
+      <c r="O1" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="38" t="s">
+      <c r="P1" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="38" t="s">
+      <c r="Q1" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="38" t="s">
+      <c r="R1" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="38" t="s">
+      <c r="S1" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="38" t="s">
+      <c r="T1" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="38" t="s">
+      <c r="U1" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="38" t="s">
+      <c r="V1" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="38" t="s">
+      <c r="W1" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="38" t="s">
+      <c r="X1" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="38" t="s">
+      <c r="Y1" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="38" t="s">
+      <c r="Z1" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="38" t="s">
+      <c r="AA1" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="38" t="s">
+      <c r="AB1" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="38" t="s">
+      <c r="AC1" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="38" t="s">
+      <c r="AD1" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="38" t="s">
+      <c r="AE1" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="38" t="s">
+      <c r="AF1" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="38" t="s">
+      <c r="AG1" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="38" t="s">
+      <c r="AH1" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="38" t="s">
+      <c r="AI1" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="38" t="s">
+      <c r="AJ1" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="38" t="s">
+      <c r="AK1" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="38" t="s">
+      <c r="AL1" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="38" t="s">
+      <c r="AM1" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="38" t="s">
+      <c r="AN1" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="38" t="s">
+      <c r="AO1" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="38" t="s">
+      <c r="AP1" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="38" t="s">
+      <c r="AQ1" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="38" t="s">
+      <c r="AR1" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="38" t="s">
+      <c r="AS1" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="38" t="s">
+      <c r="AT1" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="38" t="s">
+      <c r="AU1" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="38" t="s">
+      <c r="AV1" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="38" t="s">
+      <c r="AW1" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="38" t="s">
+      <c r="AX1" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="38" t="s">
+      <c r="AY1" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="38" t="s">
+      <c r="AZ1" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="38" t="s">
+      <c r="BA1" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="38" t="s">
+      <c r="BB1" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="38" t="s">
+      <c r="BC1" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="38" t="s">
+      <c r="BD1" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="38" t="s">
+      <c r="BE1" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" s="38" t="s">
+      <c r="BF1" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="38" t="s">
+      <c r="BG1" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="38" t="s">
+      <c r="BH1" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" s="38" t="s">
+      <c r="BI1" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" s="38" t="s">
+      <c r="BJ1" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" s="38" t="s">
+      <c r="BK1" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" s="38" t="s">
+      <c r="BL1" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" s="38" t="s">
+      <c r="BM1" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" s="38" t="s">
+      <c r="BN1" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" s="38" t="s">
+      <c r="BO1" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" s="38" t="s">
+      <c r="BP1" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" s="38" t="s">
+      <c r="BQ1" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" s="38" t="s">
+      <c r="BR1" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="BS1" s="38" t="s">
+      <c r="BS1" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="BT1" s="38" t="s">
+      <c r="BT1" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="BU1" s="38" t="s">
+      <c r="BU1" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="BV1" s="38" t="s">
+      <c r="BV1" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="BW1" s="38" t="s">
+      <c r="BW1" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="BX1" s="38" t="s">
+      <c r="BX1" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="BY1" s="38" t="s">
+      <c r="BY1" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="BZ1" s="38" t="s">
+      <c r="BZ1" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="CA1" s="38" t="s">
+      <c r="CA1" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="CB1" s="38" t="s">
+      <c r="CB1" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="CC1" s="38" t="s">
+      <c r="CC1" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="CD1" s="38" t="s">
+      <c r="CD1" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="CE1" s="39" t="s">
+      <c r="CE1" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="CF1" s="39" t="s">
+      <c r="CF1" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="CG1" s="38" t="s">
+      <c r="CG1" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="CH1" s="40" t="s">
+      <c r="CH1" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="CI1" s="38" t="s">
+      <c r="CI1" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="CJ1" s="41" t="s">
+      <c r="CJ1" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="CK1" s="38" t="s">
+      <c r="CK1" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="CL1" s="38" t="s">
+      <c r="CL1" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="CM1" s="38" t="s">
+      <c r="CM1" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="CN1" s="38" t="s">
+      <c r="CN1" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="CO1" s="38" t="s">
+      <c r="CO1" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="CP1" s="38" t="s">
+      <c r="CP1" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="CQ1" s="37" t="s">
+      <c r="CQ1" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="CR1" s="37" t="s">
+      <c r="CR1" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="CS1" s="42" t="s">
+      <c r="CS1" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="CT1" s="37" t="s">
+      <c r="CT1" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="CU1" s="42" t="s">
+      <c r="CU1" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="CV1" s="37" t="s">
+      <c r="CV1" s="38" t="s">
         <v>99</v>
+      </c>
+      <c r="CW1" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="CX1" s="38" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:CV1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <phoneticPr fontId="13" type="noConversion"/>
+  <autoFilter ref="A1:CV1">
+    <extLst/>
+  </autoFilter>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CH1:CH1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CK2:CK1048576">
+      <formula1>"正式报告,补充报告,正式报告-不报,补充报告-不报"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CH$1:CH$1048576">
       <formula1>"P,LP,不报-验证为假,不报-合并后非烈性,不报-常见假点,不报-库内降级为VUS"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CK2:CK1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
-      <formula1>"正式报告,补充报告,正式报告-不报,补充报告-不报"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:AP1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="8.5" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="2" max="2" width="8.625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
@@ -1896,7 +2477,7 @@
     <col min="40" max="40" width="10.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:42">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1907,67 +2488,67 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G1" s="35" t="s">
-        <v>103</v>
-      </c>
-      <c r="H1" s="35" t="s">
         <v>104</v>
       </c>
+      <c r="G1" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>106</v>
+      </c>
       <c r="I1" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="O1" s="36" t="s">
-        <v>111</v>
-      </c>
-      <c r="P1" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="O1" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="P1" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q1" s="37" t="s">
         <v>90</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>91</v>
@@ -1976,22 +2557,22 @@
         <v>93</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="AB1" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB1" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="AC1" s="35" t="s">
-        <v>121</v>
-      </c>
-      <c r="AD1" s="35" t="s">
-        <v>122</v>
+      <c r="AC1" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="AD1" s="36" t="s">
+        <v>124</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="AG1" s="1" t="s">
         <v>79</v>
@@ -2000,19 +2581,19 @@
         <v>80</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="AJ1" s="1" t="s">
         <v>89</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AN1" s="1" t="s">
         <v>86</v>
@@ -2025,38 +2606,42 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AP1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
-  <phoneticPr fontId="13" type="noConversion"/>
+  <autoFilter ref="A1:AP1">
+    <extLst/>
+  </autoFilter>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB1">
       <formula1>"补充报告,正式报告"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD1" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD1">
       <formula1>"Hom,Het,Hemi"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE1" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE1">
       <formula1>"A,B"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF1" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF1">
       <formula1>"Pathogenic,Likely pathogenic,VUS"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="7.75" customWidth="1" outlineLevel="1"/>
     <col min="2" max="2" width="10.5" customWidth="1" outlineLevel="1"/>
@@ -2074,56 +2659,56 @@
     <col min="16" max="16" width="11.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:19">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="33" t="s">
-        <v>129</v>
-      </c>
-      <c r="G1" s="33" t="s">
-        <v>130</v>
-      </c>
-      <c r="H1" s="33" t="s">
+      <c r="F1" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="G1" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="H1" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="I1" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="J1" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="M1" s="34" t="s">
+      <c r="K1" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="N1" s="34" t="s">
+      <c r="L1" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="O1" s="34" t="s">
+      <c r="M1" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="N1" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="O1" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="P1" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="Q1" s="33" t="s">
+      <c r="Q1" s="34" t="s">
         <v>93</v>
       </c>
       <c r="R1" t="s">
@@ -2134,21 +2719,24 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S1" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
-  <phoneticPr fontId="13" type="noConversion"/>
+  <autoFilter ref="A1:S1">
+    <extLst/>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="V1" sqref="A1:V1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="9.125" customWidth="1"/>
     <col min="2" max="2" width="14.5" customWidth="1"/>
@@ -2165,89 +2753,94 @@
     <col min="14" max="14" width="12.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="29" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="29" t="s">
+    <row r="1" s="30" customFormat="1" spans="1:22">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="G1" s="29" t="s">
-        <v>140</v>
-      </c>
-      <c r="H1" s="30" t="s">
+      <c r="F1" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="G1" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="H1" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="I1" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="L1" s="29" t="s">
+      <c r="J1" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="M1" s="30" t="s">
+      <c r="K1" s="32" t="s">
         <v>146</v>
       </c>
-      <c r="N1" s="29" t="s">
+      <c r="L1" s="30" t="s">
         <v>147</v>
       </c>
-      <c r="O1" s="31" t="s">
+      <c r="M1" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="P1" s="30" t="s">
+      <c r="N1" s="30" t="s">
         <v>149</v>
       </c>
-      <c r="Q1" s="30" t="s">
+      <c r="O1" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="R1" s="29" t="s">
+      <c r="P1" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="S1" s="32" t="s">
+      <c r="Q1" s="31" t="s">
         <v>152</v>
       </c>
-      <c r="T1" s="29" t="s">
+      <c r="R1" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="U1" s="29" t="s">
+      <c r="S1" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="T1" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="U1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="31" t="s">
+      <c r="V1" s="32" t="s">
         <v>86</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V1" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
-  <phoneticPr fontId="13" type="noConversion"/>
+  <autoFilter ref="A1:V1">
+    <extLst/>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="8.875" customWidth="1"/>
     <col min="2" max="2" width="11.125" customWidth="1"/>
@@ -2262,7 +2855,7 @@
     <col min="14" max="14" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2279,10 +2872,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -2294,34 +2887,37 @@
         <v>7</v>
       </c>
       <c r="K1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="L1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="M1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="29" t="s">
-        <v>158</v>
+      <c r="N1" s="30" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N1" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
-  <phoneticPr fontId="13" type="noConversion"/>
+  <autoFilter ref="A1:N1">
+    <extLst/>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:U1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="4.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.375" style="1" customWidth="1"/>
@@ -2339,60 +2935,60 @@
     <col min="18" max="21" width="9.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" s="25" customFormat="1" spans="1:22">
       <c r="A1" s="26" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="F1" s="27" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="G1" s="27" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="H1" s="27" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="I1" s="27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="J1" s="27" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="K1" s="26" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="L1" s="28" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="M1" s="28" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N1" s="26" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="O1" s="26" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="P1" s="26" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="Q1" s="26" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="R1" s="26" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="S1" s="26" t="s">
         <v>91</v>
@@ -2401,25 +2997,29 @@
         <v>93</v>
       </c>
       <c r="U1" s="26" t="s">
-        <v>177</v>
+        <v>179</v>
+      </c>
+      <c r="V1" s="29" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:CJ35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="11.125" customWidth="1"/>
     <col min="2" max="2" width="11.375" customWidth="1"/>
@@ -2430,7 +3030,7 @@
     <col min="10" max="10" width="11.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:88">
       <c r="A1" s="21"/>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -2520,7 +3120,7 @@
       <c r="CI1" s="21"/>
       <c r="CJ1" s="21"/>
     </row>
-    <row r="2" spans="1:88" s="20" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" s="20" customFormat="1" ht="20.25" customHeight="1" spans="1:88">
       <c r="A2" s="22"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -2610,7 +3210,7 @@
       <c r="CI2" s="24"/>
       <c r="CJ2" s="24"/>
     </row>
-    <row r="3" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:88">
       <c r="A3" s="21"/>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
@@ -2700,7 +3300,7 @@
       <c r="CI3" s="21"/>
       <c r="CJ3" s="21"/>
     </row>
-    <row r="4" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:88">
       <c r="A4" s="21"/>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
@@ -2790,7 +3390,7 @@
       <c r="CI4" s="21"/>
       <c r="CJ4" s="21"/>
     </row>
-    <row r="5" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:88">
       <c r="A5" s="21"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
@@ -2880,7 +3480,7 @@
       <c r="CI5" s="21"/>
       <c r="CJ5" s="21"/>
     </row>
-    <row r="6" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:88">
       <c r="A6" s="21"/>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
@@ -2970,7 +3570,7 @@
       <c r="CI6" s="21"/>
       <c r="CJ6" s="21"/>
     </row>
-    <row r="7" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:88">
       <c r="A7" s="21"/>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
@@ -3060,7 +3660,7 @@
       <c r="CI7" s="21"/>
       <c r="CJ7" s="21"/>
     </row>
-    <row r="8" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:88">
       <c r="A8" s="21"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
@@ -3150,7 +3750,7 @@
       <c r="CI8" s="21"/>
       <c r="CJ8" s="21"/>
     </row>
-    <row r="9" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:88">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
@@ -3240,7 +3840,7 @@
       <c r="CI9" s="21"/>
       <c r="CJ9" s="21"/>
     </row>
-    <row r="10" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:88">
       <c r="A10" s="21"/>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
@@ -3330,7 +3930,7 @@
       <c r="CI10" s="21"/>
       <c r="CJ10" s="21"/>
     </row>
-    <row r="11" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:88">
       <c r="A11" s="21"/>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
@@ -3420,7 +4020,7 @@
       <c r="CI11" s="21"/>
       <c r="CJ11" s="21"/>
     </row>
-    <row r="12" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:88">
       <c r="A12" s="21"/>
       <c r="B12" s="21"/>
       <c r="C12" s="21"/>
@@ -3510,7 +4110,7 @@
       <c r="CI12" s="21"/>
       <c r="CJ12" s="21"/>
     </row>
-    <row r="13" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:88">
       <c r="A13" s="21"/>
       <c r="B13" s="21"/>
       <c r="C13" s="21"/>
@@ -3600,7 +4200,7 @@
       <c r="CI13" s="21"/>
       <c r="CJ13" s="21"/>
     </row>
-    <row r="14" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:88">
       <c r="A14" s="21"/>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
@@ -3690,7 +4290,7 @@
       <c r="CI14" s="21"/>
       <c r="CJ14" s="21"/>
     </row>
-    <row r="15" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:88">
       <c r="A15" s="21"/>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
@@ -3780,7 +4380,7 @@
       <c r="CI15" s="21"/>
       <c r="CJ15" s="21"/>
     </row>
-    <row r="16" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:88">
       <c r="A16" s="21"/>
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
@@ -3870,7 +4470,7 @@
       <c r="CI16" s="21"/>
       <c r="CJ16" s="21"/>
     </row>
-    <row r="17" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:88">
       <c r="A17" s="21"/>
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
@@ -3960,7 +4560,7 @@
       <c r="CI17" s="21"/>
       <c r="CJ17" s="21"/>
     </row>
-    <row r="18" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:88">
       <c r="A18" s="21"/>
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
@@ -4050,7 +4650,7 @@
       <c r="CI18" s="21"/>
       <c r="CJ18" s="21"/>
     </row>
-    <row r="19" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:88">
       <c r="A19" s="21"/>
       <c r="B19" s="21"/>
       <c r="C19" s="21"/>
@@ -4140,7 +4740,7 @@
       <c r="CI19" s="21"/>
       <c r="CJ19" s="21"/>
     </row>
-    <row r="20" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:88">
       <c r="A20" s="21"/>
       <c r="B20" s="21"/>
       <c r="C20" s="21"/>
@@ -4230,7 +4830,7 @@
       <c r="CI20" s="21"/>
       <c r="CJ20" s="21"/>
     </row>
-    <row r="21" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:88">
       <c r="A21" s="21"/>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
@@ -4320,7 +4920,7 @@
       <c r="CI21" s="21"/>
       <c r="CJ21" s="21"/>
     </row>
-    <row r="22" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:88">
       <c r="A22" s="21"/>
       <c r="B22" s="21"/>
       <c r="C22" s="21"/>
@@ -4410,7 +5010,7 @@
       <c r="CI22" s="21"/>
       <c r="CJ22" s="21"/>
     </row>
-    <row r="23" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:88">
       <c r="A23" s="21"/>
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
@@ -4500,7 +5100,7 @@
       <c r="CI23" s="21"/>
       <c r="CJ23" s="21"/>
     </row>
-    <row r="24" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:88">
       <c r="A24" s="21"/>
       <c r="B24" s="21"/>
       <c r="C24" s="21"/>
@@ -4590,7 +5190,7 @@
       <c r="CI24" s="21"/>
       <c r="CJ24" s="21"/>
     </row>
-    <row r="25" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:88">
       <c r="A25" s="21"/>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
@@ -4680,7 +5280,7 @@
       <c r="CI25" s="21"/>
       <c r="CJ25" s="21"/>
     </row>
-    <row r="26" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:88">
       <c r="A26" s="21"/>
       <c r="B26" s="21"/>
       <c r="C26" s="21"/>
@@ -4770,7 +5370,7 @@
       <c r="CI26" s="21"/>
       <c r="CJ26" s="21"/>
     </row>
-    <row r="27" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:88">
       <c r="A27" s="21"/>
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
@@ -4860,7 +5460,7 @@
       <c r="CI27" s="21"/>
       <c r="CJ27" s="21"/>
     </row>
-    <row r="28" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:88">
       <c r="A28" s="21"/>
       <c r="B28" s="21"/>
       <c r="C28" s="21"/>
@@ -4950,7 +5550,7 @@
       <c r="CI28" s="21"/>
       <c r="CJ28" s="21"/>
     </row>
-    <row r="29" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:88">
       <c r="A29" s="21"/>
       <c r="B29" s="21"/>
       <c r="C29" s="21"/>
@@ -5040,7 +5640,7 @@
       <c r="CI29" s="21"/>
       <c r="CJ29" s="21"/>
     </row>
-    <row r="30" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:88">
       <c r="A30" s="21"/>
       <c r="B30" s="21"/>
       <c r="C30" s="21"/>
@@ -5130,7 +5730,7 @@
       <c r="CI30" s="21"/>
       <c r="CJ30" s="21"/>
     </row>
-    <row r="31" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:88">
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
@@ -5220,7 +5820,7 @@
       <c r="CI31" s="21"/>
       <c r="CJ31" s="21"/>
     </row>
-    <row r="32" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:88">
       <c r="A32" s="21"/>
       <c r="B32" s="21"/>
       <c r="C32" s="21"/>
@@ -5310,7 +5910,7 @@
       <c r="CI32" s="21"/>
       <c r="CJ32" s="21"/>
     </row>
-    <row r="33" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:88">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
@@ -5400,7 +6000,7 @@
       <c r="CI33" s="21"/>
       <c r="CJ33" s="21"/>
     </row>
-    <row r="34" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:88">
       <c r="A34" s="21"/>
       <c r="B34" s="21"/>
       <c r="C34" s="21"/>
@@ -5490,7 +6090,7 @@
       <c r="CI34" s="21"/>
       <c r="CJ34" s="21"/>
     </row>
-    <row r="35" spans="1:88" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:88">
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
       <c r="C35" s="21"/>
@@ -5581,41 +6181,43 @@
       <c r="CJ35" s="21"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="13" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z1:Z2" xr:uid="{00000000-0002-0000-0600-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z1:Z2">
       <formula1>"有,无"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:Y7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6"/>
   <cols>
     <col min="1" max="1" width="16.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.875" style="1" customWidth="1"/>
@@ -5627,117 +6229,117 @@
     <col min="8" max="8" width="17.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" ht="24" customHeight="1" spans="1:25">
       <c r="A1" s="2" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="Q1" s="11"/>
       <c r="R1" s="12" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="S1" s="13" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="T1" s="14" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="U1" s="15" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="V1" s="16" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="W1" s="17" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="X1" s="18" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="Y1" s="19" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="E2" s="8"/>
       <c r="F2" s="9"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="E3" s="8"/>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="E4" s="8"/>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="E5" s="8"/>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="E6" s="8"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -5745,21 +6347,23 @@
       <c r="F7" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Y1" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
-  <phoneticPr fontId="13" type="noConversion"/>
+  <autoFilter ref="A1:Y1">
+    <extLst/>
+  </autoFilter>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="4" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="3" priority="14"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="15"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="16"/>
     <cfRule type="duplicateValues" dxfId="0" priority="17"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X1" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X1">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
:bento:add 包装疾病分类 to template
</commit_message>
<xml_diff>
--- a/template/NBS-final.result-批次号_产品编号.xlsx
+++ b/template/NBS-final.result-批次号_产品编号.xlsx
@@ -4,27 +4,30 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12540" tabRatio="693"/>
+    <workbookView windowWidth="28125" windowHeight="12540" tabRatio="693"/>
   </bookViews>
   <sheets>
     <sheet name="All variants data" sheetId="1" r:id="rId1"/>
-    <sheet name="CNV" sheetId="2" r:id="rId2"/>
-    <sheet name="补充实验" sheetId="3" r:id="rId3"/>
-    <sheet name="个特" sheetId="8" r:id="rId4"/>
-    <sheet name="基因ID" sheetId="9" r:id="rId5"/>
-    <sheet name="QC" sheetId="4" r:id="rId6"/>
-    <sheet name="样本信息" sheetId="5" r:id="rId7"/>
-    <sheet name="bam文件路径" sheetId="6" r:id="rId8"/>
-    <sheet name="任务单" sheetId="7" r:id="rId9"/>
+    <sheet name="CNV" sheetId="11" r:id="rId2"/>
+    <sheet name="DMD-lumpy" sheetId="2" r:id="rId3"/>
+    <sheet name="DMD-nator" sheetId="10" r:id="rId4"/>
+    <sheet name="补充实验" sheetId="3" r:id="rId5"/>
+    <sheet name="个特" sheetId="8" r:id="rId6"/>
+    <sheet name="基因ID" sheetId="9" r:id="rId7"/>
+    <sheet name="药物检测结果" sheetId="12" r:id="rId8"/>
+    <sheet name="QC" sheetId="4" r:id="rId9"/>
+    <sheet name="样本信息" sheetId="5" r:id="rId10"/>
+    <sheet name="bam文件路径" sheetId="6" r:id="rId11"/>
+    <sheet name="任务单" sheetId="7" r:id="rId12"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'All variants data'!$A$1:$CV$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CNV!$A$1:$AP$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">补充实验!$A$1:$S$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">个特!$A$1:$V$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">基因ID!$A$1:$N$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">任务单!$A$1:$Y$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">QC!#REF!</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'All variants data'!$A$1:$CW$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'DMD-lumpy'!$A$1:$AC$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">补充实验!$A$1:$U$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">个特!$A$1:$V$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">基因ID!$A$1:$N$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">任务单!$A$1:$Y$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">QC!#REF!</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -66,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="259">
   <si>
     <t>期数</t>
   </si>
@@ -395,6 +398,9 @@
     <t>报告类别</t>
   </si>
   <si>
+    <t>包装疾病分类</t>
+  </si>
+  <si>
     <t>解读备注</t>
   </si>
   <si>
@@ -503,6 +509,114 @@
     <t>英文-突变详情</t>
   </si>
   <si>
+    <t>Chr</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>CNV_type</t>
+  </si>
+  <si>
+    <t>Gene</t>
+  </si>
+  <si>
+    <t>Gene_num</t>
+  </si>
+  <si>
+    <t>Gene_num_score</t>
+  </si>
+  <si>
+    <t>OMIM_Gene</t>
+  </si>
+  <si>
+    <t>OMIM_EX</t>
+  </si>
+  <si>
+    <t>OMIM_Phenotype</t>
+  </si>
+  <si>
+    <t>Clinvar_Pathogenic</t>
+  </si>
+  <si>
+    <t>Clinvar_Benign</t>
+  </si>
+  <si>
+    <t>Pathogenicity</t>
+  </si>
+  <si>
+    <t>Pathogenicity summary</t>
+  </si>
+  <si>
+    <t>Decipher link</t>
+  </si>
+  <si>
+    <t>22D27884697</t>
+  </si>
+  <si>
+    <t>chrX</t>
+  </si>
+  <si>
+    <t>deletion</t>
+  </si>
+  <si>
+    <t>DMD</t>
+  </si>
+  <si>
+    <t>DMD_EX48-EX50,</t>
+  </si>
+  <si>
+    <t>Becker muscular dystrophy\Duchenne muscular dystrophy\Cardiomyopathy, dilated, 3B</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/clinvar/variation/253594 [Pathogenic 0.89803];https://www.ncbi.nlm.nih.gov/clinvar/variation/253476 [Pathogenic 0.78903];https://www.ncbi.nlm.nih.gov/clinvar/variation/59260 [Pathogenic 0.76952];https://www.ncbi.nlm.nih.gov/clinvar/variation/145359 [Pathogenic 0.69565];https://www.ncbi.nlm.nih.gov/clinvar/variation/145357 [Pathogenic 0.69565];https://www.ncbi.nlm.nih.gov/clinvar/variation/253586 [Pathogenic 0.69091];https://www.ncbi.nlm.nih.gov/clinvar/variation/397200 [Likely pathogenic 0.47038];https://www.ncbi.nlm.nih.gov/clinvar/variation/153319 [Pathogenic 0.44621];https://www.ncbi.nlm.nih.gov/clinvar/variation/59256 [Pathogenic 0.43468];https://www.ncbi.nlm.nih.gov/clinvar/variation/443949 [Pathogenic 0.39271];https://www.ncbi.nlm.nih.gov/clinvar/variation/147812 [Pathogenic 0.37623];https://www.ncbi.nlm.nih.gov/clinvar/variation/145146 [Pathogenic 0.26964];https://www.ncbi.nlm.nih.gov/clinvar/variation/152267 [Pathogenic 0.17129];https://www.ncbi.nlm.nih.gov/clinvar/variation/148275 [Pathogenic 0.13822];https://www.ncbi.nlm.nih.gov/clinvar/variation/145344 [Pathogenic 0.09423];https://www.ncbi.nlm.nih.gov/clinvar/variation/149580 [Pathogenic 0.09355];https://www.ncbi.nlm.nih.gov/clinvar/variation/443414 [Pathogenic 0.08512];https://www.ncbi.nlm.nih.gov/clinvar/variation/147348 [Pathogenic 0.03529];https://www.ncbi.nlm.nih.gov/clinvar/variation/59258 [Pathogenic 0.02296];https://www.ncbi.nlm.nih.gov/clinvar/variation/59241 [Pathogenic 0.00861];https://www.ncbi.nlm.nih.gov/clinvar/variation/155429 [Pathogenic 0.00392];https://www.ncbi.nlm.nih.gov/clinvar/variation/443634 [Pathogenic 0.00392];https://www.ncbi.nlm.nih.gov/clinvar/variation/253489 [Pathogenic 0.00392];https://www.ncbi.nlm.nih.gov/clinvar/variation/146239 [Pathogenic 0.00387];https://www.ncbi.nlm.nih.gov/clinvar/variation/145973 [Pathogenic 0.00378];https://www.ncbi.nlm.nih.gov/clinvar/variation/148957 [Pathogenic 0.00376];https://www.ncbi.nlm.nih.gov/clinvar/variation/442790 [Pathogenic 0.00375];https://www.ncbi.nlm.nih.gov/clinvar/variation/145979 [Pathogenic 0.00305];https://www.ncbi.nlm.nih.gov/clinvar/variation/59181 [Pathogenic 0.00291];https://www.ncbi.nlm.nih.gov/clinvar/variation/148339 [Pathogenic 0.00286];https://www.ncbi.nlm.nih.gov/clinvar/variation/148082 [Pathogenic 0.00286];https://www.ncbi.nlm.nih.gov/clinvar/variation/144263 [Pathogenic 0.00281];https://www.ncbi.nlm.nih.gov/clinvar/variation/153302 [Pathogenic 0.00281];https://www.ncbi.nlm.nih.gov/clinvar/variation/153753 [Pathogenic 0.00273];https://www.ncbi.nlm.nih.gov/clinvar/variation/148356 [Pathogenic 0.00271];https://www.ncbi.nlm.nih.gov/clinvar/variation/148018 [Pathogenic 0.0027];https://www.ncbi.nlm.nih.gov/clinvar/variation/396610 [Pathogenic 0.00267];https://www.ncbi.nlm.nih.gov/clinvar/variation/144335 [Pathogenic 0.00265];https://www.ncbi.nlm.nih.gov/clinvar/variation/57339 [Pathogenic 0.00265];https://www.ncbi.nlm.nih.gov/clinvar/variation/155281 [Pathogenic 0.00264];https://www.ncbi.nlm.nih.gov/clinvar/variation/152052 [Pathogenic 0.00261];https://www.ncbi.nlm.nih.gov/clinvar/variation/443028 [Pathogenic 0.00255];https://www.ncbi.nlm.nih.gov/clinvar/variation/442162 [Pathogenic 0.00254];https://www.ncbi.nlm.nih.gov/clinvar/variation/396392 [Pathogenic 0.00253];https://www.ncbi.nlm.nih.gov/clinvar/variation/59202 [Pathogenic 0.00253];https://www.ncbi.nlm.nih.gov/clinvar/variation/155063 [Pathogenic 0.00249];https://www.ncbi.nlm.nih.gov/clinvar/variation/396501 [Pathogenic 0.00248];https://www.ncbi.nlm.nih.gov/clinvar/variation/59186 [Pathogenic 0.00245];https://www.ncbi.nlm.nih.gov/clinvar/variation/441968 [Pathogenic 0.00245];https://www.ncbi.nlm.nih.gov/clinvar/variation/442067 [Pathogenic 0.00244];https://www.ncbi.nlm.nih.gov/clinvar/variation/441856 [Pathogenic 0.00243];https://www.ncbi.nlm.nih.gov/clinvar/variation/59190 [Pathogenic 0.00241];https://www.ncbi.nlm.nih.gov/clinvar/variation/253571 [Pathogenic 0.00241];https://www.ncbi.nlm.nih.gov/clinvar/variation/148478 [Pathogenic 0.00241];https://www.ncbi.nlm.nih.gov/clinvar/variation/395975 [Pathogenic 0.00241];https://www.ncbi.nlm.nih.gov/clinvar/variation/144544 [Pathogenic 0.00241];https://www.ncbi.nlm.nih.gov/clinvar/variation/443322 [Pathogenic 0.0024];https://www.ncbi.nlm.nih.gov/clinvar/variation/150498 [Pathogenic 0.00239];https://www.ncbi.nlm.nih.gov/clinvar/variation/145166 [Pathogenic 0.00226];https://www.ncbi.nlm.nih.gov/clinvar/variation/154249 [Pathogenic 0.00214];https://www.ncbi.nlm.nih.gov/clinvar/variation/442354 [Pathogenic 0.00188];https://www.ncbi.nlm.nih.gov/clinvar/variation/150510 [Pathogenic 0.0016];https://www.ncbi.nlm.nih.gov/clinvar/variation/59200 [Pathogenic 0.00141];https://www.ncbi.nlm.nih.gov/clinvar/variation/148821 [Pathogenic 0.00133];https://www.ncbi.nlm.nih.gov/clinvar/variation/443946 [Pathogenic 0.00125];https://www.ncbi.nlm.nih.gov/clinvar/variation/443504 [Pathogenic 0.00113];https://www.ncbi.nlm.nih.gov/clinvar/variation/146857 [Pathogenic 0.0011];https://www.ncbi.nlm.nih.gov/clinvar/variation/149705 [Pathogenic 0.00108];https://www.ncbi.nlm.nih.gov/clinvar/variation/442724 [Pathogenic 0.00093];https://www.ncbi.nlm.nih.gov/clinvar/variation/396269 [Pathogenic 0.00092];https://www.ncbi.nlm.nih.gov/clinvar/variation/150422 [Pathogenic 0.00091];https://www.ncbi.nlm.nih.gov/clinvar/variation/396924 [Pathogenic 0.00091];https://www.ncbi.nlm.nih.gov/clinvar/variation/397461 [Pathogenic 0.0009];https://www.ncbi.nlm.nih.gov/clinvar/variation/253492 [Pathogenic 0.0009];https://www.ncbi.nlm.nih.gov/clinvar/variation/160890 [Pathogenic 0.0009];https://www.ncbi.nlm.nih.gov/clinvar/variation/144310 [Pathogenic 0.0009];https://www.ncbi.nlm.nih.gov/clinvar/variation/57161 [Pathogenic 0.0009];https://www.ncbi.nlm.nih.gov/clinvar/variation/145995 [Pathogenic 0.0009];https://www.ncbi.nlm.nih.gov/clinvar/variation/144465 [Pathogenic 0.0009];https://www.ncbi.nlm.nih.gov/clinvar/variation/155374 [Pathogenic 0.0009];https://www.ncbi.nlm.nih.gov/clinvar/variation/161088 [Pathogenic 0.0009];https://www.ncbi.nlm.nih.gov/clinvar/variation/395687 [Pathogenic 0.0009];https://www.ncbi.nlm.nih.gov/clinvar/variation/146861 [Pathogenic 0.0009];https://www.ncbi.nlm.nih.gov/clinvar/variation/57087 [Pathogenic 0.0009];https://www.ncbi.nlm.nih.gov/clinvar/variation/160983 [Pathogenic 0.0009];https://www.ncbi.nlm.nih.gov/clinvar/variation/394013 [Pathogenic 0.0009];https://www.ncbi.nlm.nih.gov/clinvar/variation/394672 [Pathogenic 0.0009];https://www.ncbi.nlm.nih.gov/clinvar/variation/147257 [Pathogenic 0.0009];https://www.ncbi.nlm.nih.gov/clinvar/variation/395718 [Pathogenic 0.0009];https://www.ncbi.nlm.nih.gov/clinvar/variation/253495 [Pathogenic 0.0009];https://www.ncbi.nlm.nih.gov/clinvar/variation/161089 [Pathogenic 0.0009];https://www.ncbi.nlm.nih.gov/clinvar/variation/396669 [Pathogenic 0.0009];https://www.ncbi.nlm.nih.gov/clinvar/variation/146764 [Pathogenic 0.0009]</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/clinvar/variation/148345 [Likely benign 0.67774];https://www.ncbi.nlm.nih.gov/clinvar/variation/148358 [Likely benign 0.50638];https://www.ncbi.nlm.nih.gov/clinvar/variation/148205 [Likely benign 0.50638];https://www.ncbi.nlm.nih.gov/clinvar/variation/442954 [Likely benign 0.37719];https://www.ncbi.nlm.nih.gov/clinvar/variation/153850 [Likely benign 0.31827]</t>
+  </si>
+  <si>
+    <t>Clinvar:Pathogenic</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>https://decipher.sanger.ac.uk/browser#q/X:31794001-31934000%20/location/X:31794001-31934000</t>
+  </si>
+  <si>
+    <t>CHROM</t>
+  </si>
+  <si>
+    <t>POS</t>
+  </si>
+  <si>
+    <t>END</t>
+  </si>
+  <si>
+    <t>SVTYPE</t>
+  </si>
+  <si>
+    <t>SU</t>
+  </si>
+  <si>
+    <t>RATIO</t>
+  </si>
+  <si>
+    <t>OMIM_exon</t>
+  </si>
+  <si>
+    <t>DEL</t>
+  </si>
+  <si>
+    <t>Duchenne muscular dystrophy\Becker muscular dystrophy\Cardiomyopathy, dilated, 3B</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/clinvar/variation/253594 [Pathogenic 0.89];https://www.ncbi.nlm.nih.gov/clinvar/variation/253476 [Pathogenic 0.79];https://www.ncbi.nlm.nih.gov/clinvar/variation/59260 [Pathogenic 0.77];https://www.ncbi.nlm.nih.gov/clinvar/variation/145357 [Pathogenic 0.7];https://www.ncbi.nlm.nih.gov/clinvar/variation/145359 [Pathogenic 0.7];https://www.ncbi.nlm.nih.gov/clinvar/variation/253586 [Pathogenic 0.69];https://www.ncbi.nlm.nih.gov/clinvar/variation/397200 [Likely pathogenic 0.47];https://www.ncbi.nlm.nih.gov/clinvar/variation/153319 [Pathogenic 0.45];https://www.ncbi.nlm.nih.gov/clinvar/variation/59256 [Pathogenic 0.43];https://www.ncbi.nlm.nih.gov/clinvar/variation/443949 [Pathogenic 0.39];https://www.ncbi.nlm.nih.gov/clinvar/variation/147812 [Pathogenic 0.38];https://www.ncbi.nlm.nih.gov/clinvar/variation/145146 [Pathogenic 0.27];https://www.ncbi.nlm.nih.gov/clinvar/variation/152267 [Pathogenic 0.17];https://www.ncbi.nlm.nih.gov/clinvar/variation/148275 [Pathogenic 0.14];https://www.ncbi.nlm.nih.gov/clinvar/variation/149580 [Pathogenic 0.09];https://www.ncbi.nlm.nih.gov/clinvar/variation/145344 [Pathogenic 0.09];https://www.ncbi.nlm.nih.gov/clinvar/variation/443414 [Pathogenic 0.08];https://www.ncbi.nlm.nih.gov/clinvar/variation/147348 [Pathogenic 0.04];https://www.ncbi.nlm.nih.gov/clinvar/variation/59258 [Pathogenic 0.02];https://www.ncbi.nlm.nih.gov/clinvar/variation/59241 [Pathogenic 0.01];https://www.ncbi.nlm.nih.gov/clinvar/variation/396924 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/395718 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/145995 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/443504 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/150498 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/144263 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/146239 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/253489 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/59186 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/160890 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/148957 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/148821 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/441856 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/253571 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/443028 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/149705 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/155429 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/59190 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/395975 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/443946 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/144335 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/161088 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/145973 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/57161 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/148082 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/144465 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/59202 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/155063 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/155281 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/148356 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/395687 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/442724 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/153753 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/396501 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/442067 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/57339 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/146857 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/442162 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/442790 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/253495 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/394672 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/146861 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/147257 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/441968 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/153302 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/144544 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/396610 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/161089 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/396392 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/148339 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/394013 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/144310 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/443634 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/150422 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/253492 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/396669 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/59181 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/57087 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/148478 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/145166 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/155374 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/443322 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/146764 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/160983 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/145979 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/150510 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/148018 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/59200 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/152052 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/154249 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/442354 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/396269 [Pathogenic 0];https://www.ncbi.nlm.nih.gov/clinvar/variation/397461 [Pathogenic 0]</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/clinvar/variation/148345 [Likely benign 0.68];https://www.ncbi.nlm.nih.gov/clinvar/variation/148205 [Likely benign 0.51];https://www.ncbi.nlm.nih.gov/clinvar/variation/148358 [Likely benign 0.51];https://www.ncbi.nlm.nih.gov/clinvar/variation/442954 [Likely benign 0.38];https://www.ncbi.nlm.nih.gov/clinvar/variation/153850 [Likely benign 0.32]</t>
+  </si>
+  <si>
     <t>地贫_QC</t>
   </si>
   <si>
@@ -524,6 +638,12 @@
     <t>SMN1_质控结果</t>
   </si>
   <si>
+    <t>SMN1_CN</t>
+  </si>
+  <si>
+    <t>SMN1_CN_raw</t>
+  </si>
+  <si>
     <t>SMN1 EX7 del最终结果</t>
   </si>
   <si>
@@ -593,6 +713,57 @@
     <t>是否通过质控</t>
   </si>
   <si>
+    <t>样本编号</t>
+  </si>
+  <si>
+    <t>药物分类</t>
+  </si>
+  <si>
+    <t>标签</t>
+  </si>
+  <si>
+    <t>药物名称</t>
+  </si>
+  <si>
+    <t>英文名</t>
+  </si>
+  <si>
+    <t>检测基因</t>
+  </si>
+  <si>
+    <t>影响类型</t>
+  </si>
+  <si>
+    <t>证据等级</t>
+  </si>
+  <si>
+    <t>参考基因型</t>
+  </si>
+  <si>
+    <t>Var</t>
+  </si>
+  <si>
+    <t>代谢型</t>
+  </si>
+  <si>
+    <t>分条结果说明</t>
+  </si>
+  <si>
+    <t>分条用药建议</t>
+  </si>
+  <si>
+    <t>参考来源</t>
+  </si>
+  <si>
+    <t>阳性结果说明</t>
+  </si>
+  <si>
+    <t>用药建议</t>
+  </si>
+  <si>
+    <t>结果说明</t>
+  </si>
+  <si>
     <t>Order</t>
   </si>
   <si>
@@ -677,13 +848,7 @@
     <t>flowID</t>
   </si>
   <si>
-    <t>样本编号</t>
-  </si>
-  <si>
     <t>疾病</t>
-  </si>
-  <si>
-    <t>检测基因</t>
   </si>
   <si>
     <t>产品编码</t>
@@ -739,7 +904,7 @@
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="yyyy/m/d;@"/>
   </numFmts>
-  <fonts count="33">
+  <fonts count="34">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -825,6 +990,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1039,6 +1211,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14981536301767"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1076,12 +1260,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1208,12 +1386,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1394,10 +1566,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1406,36 +1578,33 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1445,98 +1614,101 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="22" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1616,6 +1788,10 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1627,6 +1803,24 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1634,7 +1828,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1643,9 +1837,10 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1714,8 +1909,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="00FF0000"/>
       <color rgb="00FFFF00"/>
-      <color rgb="00FF0000"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2013,14 +2208,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:CX1"/>
+  <dimension ref="A1:CY1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="CK4" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="CY7" sqref="CY7"/>
+      <selection pane="bottomRight" activeCell="CS16" sqref="CS16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2092,333 +2287,337 @@
     <col min="91" max="91" width="12.625" style="1" customWidth="1"/>
     <col min="92" max="92" width="12.125" style="1" customWidth="1"/>
     <col min="93" max="93" width="12.625" style="1" customWidth="1"/>
-    <col min="94" max="94" width="11.5" style="1" customWidth="1"/>
-    <col min="95" max="95" width="12.375" customWidth="1"/>
-    <col min="96" max="96" width="13.5" customWidth="1"/>
-    <col min="97" max="97" width="11.125" customWidth="1"/>
-    <col min="98" max="98" width="12.625" customWidth="1"/>
-    <col min="99" max="99" width="11.625" customWidth="1"/>
-    <col min="100" max="100" width="15.125" customWidth="1"/>
+    <col min="94" max="94" width="13" style="1" customWidth="1"/>
+    <col min="95" max="95" width="13" customWidth="1"/>
+    <col min="96" max="96" width="15.25" customWidth="1"/>
+    <col min="97" max="97" width="13.5" customWidth="1"/>
+    <col min="98" max="98" width="11.125" customWidth="1"/>
+    <col min="99" max="99" width="12.625" customWidth="1"/>
+    <col min="100" max="100" width="11.625" customWidth="1"/>
+    <col min="101" max="101" width="15.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="38" customFormat="1" ht="15" spans="1:102">
-      <c r="A1" s="39" t="s">
+    <row r="1" s="46" customFormat="1" ht="15" spans="1:103">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="39" t="s">
+      <c r="J1" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="K1" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="39" t="s">
+      <c r="L1" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="M1" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="39" t="s">
+      <c r="N1" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="O1" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="39" t="s">
+      <c r="P1" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="39" t="s">
+      <c r="Q1" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="39" t="s">
+      <c r="R1" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="39" t="s">
+      <c r="S1" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="39" t="s">
+      <c r="T1" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="39" t="s">
+      <c r="U1" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="39" t="s">
+      <c r="V1" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="39" t="s">
+      <c r="W1" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="39" t="s">
+      <c r="X1" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="39" t="s">
+      <c r="Y1" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="39" t="s">
+      <c r="Z1" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="39" t="s">
+      <c r="AA1" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="39" t="s">
+      <c r="AB1" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="39" t="s">
+      <c r="AC1" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="39" t="s">
+      <c r="AD1" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="39" t="s">
+      <c r="AE1" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="39" t="s">
+      <c r="AF1" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="39" t="s">
+      <c r="AG1" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="39" t="s">
+      <c r="AH1" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="39" t="s">
+      <c r="AI1" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="39" t="s">
+      <c r="AJ1" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="39" t="s">
+      <c r="AK1" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="39" t="s">
+      <c r="AL1" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="39" t="s">
+      <c r="AM1" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="39" t="s">
+      <c r="AN1" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="39" t="s">
+      <c r="AO1" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="39" t="s">
+      <c r="AP1" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="39" t="s">
+      <c r="AQ1" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="39" t="s">
+      <c r="AR1" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="39" t="s">
+      <c r="AS1" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="39" t="s">
+      <c r="AT1" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="39" t="s">
+      <c r="AU1" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="39" t="s">
+      <c r="AV1" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="39" t="s">
+      <c r="AW1" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="39" t="s">
+      <c r="AX1" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="39" t="s">
+      <c r="AY1" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="39" t="s">
+      <c r="AZ1" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="39" t="s">
+      <c r="BA1" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="39" t="s">
+      <c r="BB1" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="39" t="s">
+      <c r="BC1" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="39" t="s">
+      <c r="BD1" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="39" t="s">
+      <c r="BE1" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" s="39" t="s">
+      <c r="BF1" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="39" t="s">
+      <c r="BG1" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="39" t="s">
+      <c r="BH1" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" s="39" t="s">
+      <c r="BI1" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" s="39" t="s">
+      <c r="BJ1" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" s="39" t="s">
+      <c r="BK1" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" s="39" t="s">
+      <c r="BL1" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" s="39" t="s">
+      <c r="BM1" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" s="39" t="s">
+      <c r="BN1" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" s="39" t="s">
+      <c r="BO1" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" s="39" t="s">
+      <c r="BP1" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" s="39" t="s">
+      <c r="BQ1" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" s="39" t="s">
+      <c r="BR1" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="BS1" s="39" t="s">
+      <c r="BS1" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="BT1" s="39" t="s">
+      <c r="BT1" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="BU1" s="39" t="s">
+      <c r="BU1" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="BV1" s="39" t="s">
+      <c r="BV1" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="BW1" s="39" t="s">
+      <c r="BW1" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="BX1" s="39" t="s">
+      <c r="BX1" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="BY1" s="39" t="s">
+      <c r="BY1" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="BZ1" s="39" t="s">
+      <c r="BZ1" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="CA1" s="39" t="s">
+      <c r="CA1" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="CB1" s="39" t="s">
+      <c r="CB1" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="CC1" s="39" t="s">
+      <c r="CC1" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="CD1" s="39" t="s">
+      <c r="CD1" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="CE1" s="40" t="s">
+      <c r="CE1" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="CF1" s="40" t="s">
+      <c r="CF1" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="CG1" s="39" t="s">
+      <c r="CG1" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="CH1" s="41" t="s">
+      <c r="CH1" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="CI1" s="39" t="s">
+      <c r="CI1" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="CJ1" s="42" t="s">
+      <c r="CJ1" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="CK1" s="39" t="s">
+      <c r="CK1" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="CL1" s="39" t="s">
+      <c r="CL1" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="CM1" s="39" t="s">
+      <c r="CM1" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="CN1" s="39" t="s">
+      <c r="CN1" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="CO1" s="39" t="s">
+      <c r="CO1" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="CP1" s="39" t="s">
+      <c r="CP1" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="CQ1" s="38" t="s">
+      <c r="CQ1" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="CR1" s="38" t="s">
+      <c r="CR1" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="CS1" s="43" t="s">
+      <c r="CS1" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="CT1" s="38" t="s">
+      <c r="CT1" s="52" t="s">
         <v>97</v>
       </c>
-      <c r="CU1" s="43" t="s">
+      <c r="CU1" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="CV1" s="38" t="s">
+      <c r="CV1" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="CW1" s="38" t="s">
+      <c r="CW1" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="CX1" s="38" t="s">
+      <c r="CX1" s="46" t="s">
         <v>101</v>
+      </c>
+      <c r="CY1" s="46" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:CV1">
+  <autoFilter ref="A1:CW1">
     <extLst/>
   </autoFilter>
   <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CH$1:CH$1048576">
+      <formula1>"P,LP,不报-验证为假,不报-合并后非烈性,不报-常见假点,不报-库内降级为VUS"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CK2:CK1048576">
       <formula1>"正式报告,补充报告,正式报告-不报,补充报告-不报"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CH$1:CH$1048576">
-      <formula1>"P,LP,不报-验证为假,不报-合并后非烈性,不报-常见假点,不报-库内降级为VUS"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2427,590 +2626,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:AP1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
-      <selection/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Y16" sqref="Y16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="8.5" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="2" max="2" width="8.625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="18.625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="5.25" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.25" style="1" customWidth="1"/>
-    <col min="8" max="8" width="7.625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7.875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.75" style="1" customWidth="1"/>
-    <col min="13" max="13" width="16.125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="14.75" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15.125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="15.375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="12.75" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="19" width="11.625" style="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="10.625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="5.5" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="24" width="3.375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="25" max="25" width="10.625" style="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="31" width="10.625" style="1" customWidth="1"/>
-    <col min="32" max="32" width="11.625" style="1" customWidth="1"/>
-    <col min="33" max="33" width="13.5" style="1" customWidth="1"/>
-    <col min="34" max="34" width="10.375" style="1" customWidth="1"/>
-    <col min="35" max="35" width="15.625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="36" max="36" width="15.625" style="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="10.625" style="1" customWidth="1"/>
-    <col min="38" max="38" width="15.625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="39" max="39" width="15.625" style="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="10.625" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:42">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G1" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="H1" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="O1" s="37" t="s">
-        <v>113</v>
-      </c>
-      <c r="P1" s="37" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q1" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="AB1" s="36" t="s">
-        <v>94</v>
-      </c>
-      <c r="AC1" s="36" t="s">
-        <v>123</v>
-      </c>
-      <c r="AD1" s="36" t="s">
-        <v>124</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:AP1">
-    <extLst/>
-  </autoFilter>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB1">
-      <formula1>"补充报告,正式报告"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD1">
-      <formula1>"Hom,Het,Hemi"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE1">
-      <formula1>"A,B"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF1">
-      <formula1>"Pathogenic,Likely pathogenic,VUS"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:S1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
-      <selection/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="7.75" customWidth="1" outlineLevel="1"/>
-    <col min="2" max="2" width="10.5" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="18.625" customWidth="1"/>
-    <col min="4" max="4" width="14.625" customWidth="1"/>
-    <col min="6" max="6" width="15.625" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="17.375" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="15" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="17.25" customWidth="1"/>
-    <col min="10" max="10" width="16.25" customWidth="1"/>
-    <col min="11" max="12" width="15.625" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="21.375" customWidth="1"/>
-    <col min="14" max="14" width="27.125" customWidth="1"/>
-    <col min="15" max="15" width="23.75" customWidth="1"/>
-    <col min="16" max="16" width="11.125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19">
-      <c r="A1" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="G1" s="34" t="s">
-        <v>132</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="I1" s="35" t="s">
-        <v>134</v>
-      </c>
-      <c r="J1" s="35" t="s">
-        <v>135</v>
-      </c>
-      <c r="K1" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="L1" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="M1" s="35" t="s">
-        <v>138</v>
-      </c>
-      <c r="N1" s="35" t="s">
-        <v>139</v>
-      </c>
-      <c r="O1" s="35" t="s">
-        <v>140</v>
-      </c>
-      <c r="P1" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q1" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="R1" t="s">
-        <v>95</v>
-      </c>
-      <c r="S1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:S1">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:V1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V1" sqref="A1:V1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="9.125" customWidth="1"/>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="19.875" customWidth="1"/>
-    <col min="4" max="4" width="11.75" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="10.75" customWidth="1"/>
-    <col min="8" max="8" width="15.5" customWidth="1"/>
-    <col min="9" max="9" width="13.625" customWidth="1"/>
-    <col min="10" max="10" width="17.625" customWidth="1"/>
-    <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="11.25" customWidth="1"/>
-    <col min="13" max="13" width="11.5" customWidth="1"/>
-    <col min="14" max="14" width="12.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="30" customFormat="1" spans="1:22">
-      <c r="A1" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="G1" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="H1" s="31" t="s">
-        <v>143</v>
-      </c>
-      <c r="I1" s="31" t="s">
-        <v>144</v>
-      </c>
-      <c r="J1" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="K1" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="L1" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="M1" s="31" t="s">
-        <v>148</v>
-      </c>
-      <c r="N1" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="O1" s="32" t="s">
-        <v>150</v>
-      </c>
-      <c r="P1" s="31" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q1" s="31" t="s">
-        <v>152</v>
-      </c>
-      <c r="R1" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="S1" s="33" t="s">
-        <v>154</v>
-      </c>
-      <c r="T1" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="U1" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="V1" s="32" t="s">
-        <v>86</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:V1">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:N1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="8.875" customWidth="1"/>
-    <col min="2" max="2" width="11.125" customWidth="1"/>
-    <col min="3" max="3" width="20.625" customWidth="1"/>
-    <col min="4" max="4" width="11.5" customWidth="1"/>
-    <col min="5" max="5" width="8" customWidth="1"/>
-    <col min="6" max="6" width="9.875" customWidth="1"/>
-    <col min="10" max="10" width="9.875" customWidth="1"/>
-    <col min="11" max="11" width="12.875" customWidth="1"/>
-    <col min="12" max="12" width="10.75" customWidth="1"/>
-    <col min="13" max="13" width="16.75" customWidth="1"/>
-    <col min="14" max="14" width="15.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>156</v>
-      </c>
-      <c r="G1" t="s">
-        <v>157</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>158</v>
-      </c>
-      <c r="L1" t="s">
-        <v>159</v>
-      </c>
-      <c r="M1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="30" t="s">
-        <v>160</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:N1">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:V1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="4.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.375" style="1" customWidth="1"/>
-    <col min="3" max="4" width="9.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5" style="1" customWidth="1"/>
-    <col min="6" max="9" width="9.625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.25" style="1" customWidth="1"/>
-    <col min="11" max="11" width="6.125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="7.75" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="7.375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9.625" customWidth="1"/>
-    <col min="17" max="17" width="8.625" customWidth="1"/>
-    <col min="18" max="21" width="9.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="25" customFormat="1" spans="1:22">
-      <c r="A1" s="26" t="s">
-        <v>161</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>162</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>163</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>165</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>166</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>167</v>
-      </c>
-      <c r="H1" s="27" t="s">
-        <v>168</v>
-      </c>
-      <c r="I1" s="27" t="s">
-        <v>169</v>
-      </c>
-      <c r="J1" s="27" t="s">
-        <v>170</v>
-      </c>
-      <c r="K1" s="26" t="s">
-        <v>171</v>
-      </c>
-      <c r="L1" s="28" t="s">
-        <v>172</v>
-      </c>
-      <c r="M1" s="28" t="s">
-        <v>173</v>
-      </c>
-      <c r="N1" s="26" t="s">
-        <v>174</v>
-      </c>
-      <c r="O1" s="26" t="s">
-        <v>175</v>
-      </c>
-      <c r="P1" s="26" t="s">
-        <v>176</v>
-      </c>
-      <c r="Q1" s="26" t="s">
-        <v>177</v>
-      </c>
-      <c r="R1" s="26" t="s">
-        <v>178</v>
-      </c>
-      <c r="S1" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="T1" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="U1" s="26" t="s">
-        <v>179</v>
-      </c>
-      <c r="V1" s="29" t="s">
-        <v>180</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:CJ35"/>
@@ -6192,7 +5808,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1"/>
@@ -6208,13 +5824,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:Y7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6"/>
@@ -6231,77 +5847,77 @@
   <sheetData>
     <row r="1" ht="24" customHeight="1" spans="1:25">
       <c r="A1" s="2" t="s">
-        <v>181</v>
+        <v>237</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>182</v>
+        <v>238</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>183</v>
+        <v>239</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>184</v>
+        <v>240</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>185</v>
+        <v>241</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>186</v>
+        <v>242</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>187</v>
+        <v>243</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>188</v>
+        <v>244</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>190</v>
+        <v>245</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>192</v>
+        <v>246</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>193</v>
+        <v>247</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>194</v>
+        <v>248</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>195</v>
+        <v>249</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>196</v>
+        <v>250</v>
       </c>
       <c r="Q1" s="11"/>
       <c r="R1" s="12" t="s">
-        <v>197</v>
+        <v>251</v>
       </c>
       <c r="S1" s="13" t="s">
-        <v>198</v>
+        <v>252</v>
       </c>
       <c r="T1" s="14" t="s">
-        <v>199</v>
+        <v>253</v>
       </c>
       <c r="U1" s="15" t="s">
-        <v>200</v>
+        <v>254</v>
       </c>
       <c r="V1" s="16" t="s">
-        <v>201</v>
+        <v>255</v>
       </c>
       <c r="W1" s="17" t="s">
-        <v>202</v>
+        <v>256</v>
       </c>
       <c r="X1" s="18" t="s">
-        <v>203</v>
+        <v>257</v>
       </c>
       <c r="Y1" s="19" t="s">
-        <v>204</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -6366,4 +5982,1038 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:AP1"/>
+  <sheetViews>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="8.5" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="2" width="8.625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="18.625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5.375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.25" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.25" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.75" style="1" customWidth="1"/>
+    <col min="13" max="13" width="16.125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.75" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15.375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.75" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="11.625" style="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="10.625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="5.5" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="24" width="3.375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="25" max="25" width="10.625" style="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="31" width="10.625" style="1" customWidth="1"/>
+    <col min="32" max="32" width="11.625" style="1" customWidth="1"/>
+    <col min="33" max="33" width="13.5" style="1" customWidth="1"/>
+    <col min="34" max="34" width="10.375" style="1" customWidth="1"/>
+    <col min="35" max="35" width="15.625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="36" max="36" width="15.625" style="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="10.625" style="1" customWidth="1"/>
+    <col min="38" max="38" width="15.625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="39" max="39" width="15.625" style="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="10.625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:42">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="O1" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="P1" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q1" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AB1" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC1" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="AD1" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB1">
+      <formula1>"补充报告,正式报告"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD1">
+      <formula1>"Hom,Het,Hemi"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE1">
+      <formula1>"A,B"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF1">
+      <formula1>"Pathogenic,Likely pathogenic,VUS"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:AC2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="U1" sqref="U1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="8.5" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="2" width="8.625" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="18.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.75" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.75" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.75" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.75" style="1" customWidth="1"/>
+    <col min="13" max="13" width="16.125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.75" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15.375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.75" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.375" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="11.625" style="1" customWidth="1"/>
+    <col min="20" max="21" width="23.875" style="1" customWidth="1"/>
+    <col min="22" max="22" width="15.125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="13.5" style="1" customWidth="1"/>
+    <col min="24" max="24" width="12.375" style="1" customWidth="1"/>
+    <col min="25" max="25" width="12.125" style="1" customWidth="1"/>
+    <col min="26" max="27" width="13.625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="G1" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="I1" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="J1" s="43" t="s">
+        <v>135</v>
+      </c>
+      <c r="K1" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="L1" s="43" t="s">
+        <v>137</v>
+      </c>
+      <c r="M1" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="N1" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="O1" s="43" t="s">
+        <v>140</v>
+      </c>
+      <c r="P1" s="43" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q1" s="43" t="s">
+        <v>142</v>
+      </c>
+      <c r="R1" s="43" t="s">
+        <v>143</v>
+      </c>
+      <c r="S1" s="43" t="s">
+        <v>144</v>
+      </c>
+      <c r="T1" s="43" t="s">
+        <v>145</v>
+      </c>
+      <c r="U1" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="V1" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="W1" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="4:21">
+      <c r="D2" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>147</v>
+      </c>
+      <c r="G2" s="40">
+        <v>31794001</v>
+      </c>
+      <c r="H2" s="40">
+        <v>31934000</v>
+      </c>
+      <c r="I2" s="40" t="s">
+        <v>148</v>
+      </c>
+      <c r="J2" s="40" t="s">
+        <v>149</v>
+      </c>
+      <c r="K2" s="40">
+        <v>1</v>
+      </c>
+      <c r="L2" s="40">
+        <v>0</v>
+      </c>
+      <c r="M2" s="40" t="s">
+        <v>149</v>
+      </c>
+      <c r="N2" s="40" t="s">
+        <v>150</v>
+      </c>
+      <c r="O2" s="40" t="s">
+        <v>151</v>
+      </c>
+      <c r="P2" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q2" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="R2" s="40" t="s">
+        <v>154</v>
+      </c>
+      <c r="S2" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="T2" s="40" t="s">
+        <v>156</v>
+      </c>
+      <c r="U2" s="41"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:AC2">
+    <extLst/>
+  </autoFilter>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1">
+      <formula1>"补充报告,正式报告"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W1">
+      <formula1>"Hom,Het,Hemi"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X1">
+      <formula1>"Pathogenic,Likely pathogenic,VUS"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:AA2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="6.25" customWidth="1"/>
+    <col min="2" max="2" width="8.625" customWidth="1"/>
+    <col min="3" max="3" width="8.25" customWidth="1"/>
+    <col min="4" max="4" width="11.75" customWidth="1"/>
+    <col min="12" max="12" width="10.75" customWidth="1"/>
+    <col min="13" max="13" width="15.125" customWidth="1"/>
+    <col min="14" max="14" width="13" customWidth="1"/>
+    <col min="15" max="16" width="13.25" customWidth="1"/>
+    <col min="18" max="19" width="16.125" customWidth="1"/>
+    <col min="20" max="20" width="12.125" customWidth="1"/>
+    <col min="22" max="22" width="12.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="G1" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="H1" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="I1" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="J1" s="39" t="s">
+        <v>161</v>
+      </c>
+      <c r="K1" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="L1" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="M1" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="N1" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="O1" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="P1" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q1" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="R1" s="39" t="s">
+        <v>144</v>
+      </c>
+      <c r="S1" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="T1" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="U1" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="4:19">
+      <c r="D2" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>147</v>
+      </c>
+      <c r="G2" s="40">
+        <v>31793842</v>
+      </c>
+      <c r="H2" s="40">
+        <v>31933654</v>
+      </c>
+      <c r="I2" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="J2" s="40">
+        <v>19</v>
+      </c>
+      <c r="K2" s="40">
+        <v>27.1605</v>
+      </c>
+      <c r="L2" s="40" t="s">
+        <v>149</v>
+      </c>
+      <c r="M2" s="40" t="s">
+        <v>150</v>
+      </c>
+      <c r="N2" s="40" t="s">
+        <v>165</v>
+      </c>
+      <c r="O2" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="P2" s="40" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q2" s="40" t="s">
+        <v>154</v>
+      </c>
+      <c r="R2" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="S2" s="41"/>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T1">
+      <formula1>"补充报告,正式报告"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U1">
+      <formula1>"Hom,Het,Hemi"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1">
+      <formula1>"Pathogenic,Likely pathogenic,VUS"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:U1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="7.75" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="18.625" customWidth="1"/>
+    <col min="4" max="4" width="14.625" customWidth="1"/>
+    <col min="6" max="6" width="15.625" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="17.375" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="15" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="17.25" customWidth="1"/>
+    <col min="10" max="10" width="16.25" customWidth="1"/>
+    <col min="11" max="11" width="21.125" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="12" width="20" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="14" width="15.625" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="21.375" customWidth="1"/>
+    <col min="16" max="16" width="27.125" customWidth="1"/>
+    <col min="17" max="17" width="23.75" customWidth="1"/>
+    <col min="18" max="18" width="11.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21">
+      <c r="A1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="J1" s="37" t="s">
+        <v>172</v>
+      </c>
+      <c r="K1" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="L1" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="M1" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="N1" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="O1" s="37" t="s">
+        <v>177</v>
+      </c>
+      <c r="P1" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q1" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="R1" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="S1" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="T1" t="s">
+        <v>96</v>
+      </c>
+      <c r="U1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:U1">
+    <extLst/>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:V1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V1" sqref="A1:V1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="9.125" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="19.875" customWidth="1"/>
+    <col min="4" max="4" width="11.75" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="10.75" customWidth="1"/>
+    <col min="8" max="8" width="15.5" customWidth="1"/>
+    <col min="9" max="9" width="13.625" customWidth="1"/>
+    <col min="10" max="10" width="17.625" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
+    <col min="12" max="12" width="11.25" customWidth="1"/>
+    <col min="13" max="13" width="11.5" customWidth="1"/>
+    <col min="14" max="14" width="12.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="32" customFormat="1" spans="1:22">
+      <c r="A1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="H1" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="J1" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="K1" s="34" t="s">
+        <v>185</v>
+      </c>
+      <c r="L1" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="M1" s="33" t="s">
+        <v>187</v>
+      </c>
+      <c r="N1" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="O1" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="P1" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q1" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="R1" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="S1" s="35" t="s">
+        <v>193</v>
+      </c>
+      <c r="T1" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="U1" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:V1">
+    <extLst/>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="8.875" customWidth="1"/>
+    <col min="2" max="2" width="11.125" customWidth="1"/>
+    <col min="3" max="3" width="20.625" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="6" max="6" width="9.875" customWidth="1"/>
+    <col min="10" max="10" width="9.875" customWidth="1"/>
+    <col min="11" max="11" width="12.875" customWidth="1"/>
+    <col min="12" max="12" width="10.75" customWidth="1"/>
+    <col min="13" max="13" width="16.75" customWidth="1"/>
+    <col min="14" max="14" width="15.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G1" t="s">
+        <v>196</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>197</v>
+      </c>
+      <c r="L1" t="s">
+        <v>198</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="32" t="s">
+        <v>199</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:N1">
+    <extLst/>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:T1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetData>
+    <row r="1" s="30" customFormat="1" ht="15" spans="1:20">
+      <c r="A1" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>204</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>205</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>207</v>
+      </c>
+      <c r="J1" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="K1" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="M1" s="31" t="s">
+        <v>190</v>
+      </c>
+      <c r="N1" s="31" t="s">
+        <v>210</v>
+      </c>
+      <c r="O1" s="31" t="s">
+        <v>211</v>
+      </c>
+      <c r="P1" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q1" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="R1" s="31" t="s">
+        <v>214</v>
+      </c>
+      <c r="S1" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="T1" s="31" t="s">
+        <v>216</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:V1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="4.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.375" style="1" customWidth="1"/>
+    <col min="3" max="4" width="9.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="1" customWidth="1"/>
+    <col min="6" max="9" width="9.625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.25" style="1" customWidth="1"/>
+    <col min="11" max="11" width="6.125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="7.75" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="7.375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.625" customWidth="1"/>
+    <col min="17" max="17" width="8.625" customWidth="1"/>
+    <col min="18" max="21" width="9.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="25" customFormat="1" spans="1:22">
+      <c r="A1" s="26" t="s">
+        <v>217</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>218</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="J1" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>230</v>
+      </c>
+      <c r="O1" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="P1" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q1" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="R1" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="S1" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="T1" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="U1" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="V1" s="29" t="s">
+        <v>236</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>